<commit_message>
ballast pump logic added in loading and discharging excel
</commit_message>
<xml_diff>
--- a/api/cp-dss-api/gateway/src/main/resources/reports/discharging/Vessel_1_Discharging_Plan_Template.xlsx
+++ b/api/cp-dss-api/gateway/src/main/resources/reports/discharging/Vessel_1_Discharging_Plan_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17316" windowHeight="6156" tabRatio="399" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17316" windowHeight="6156" tabRatio="399"/>
   </bookViews>
   <sheets>
     <sheet name="CRUD - 021 pg1" sheetId="27" r:id="rId1"/>
@@ -2186,6 +2186,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="E84" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="14"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:
+jx:each(items="sheetThree.ballastPumps[0].cargoTankUllage.status" var="ballastPumpStatus"  direction="RIGHT" lastCell="F84")</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E85" authorId="0" shapeId="0">
       <text>
         <r>
@@ -2197,7 +2222,7 @@
             <family val="2"/>
           </rPr>
           <t>Author:
-jx:each(items="sheetThree.ballastPumps[0].cargoTankUllage.status" var="ballastPumpStatus"  direction="RIGHT" lastCell="F85")</t>
+jx:each(items="sheetThree.ballastPumps[1].cargoTankUllage.status" var="ballastPumpStatus1"  direction="RIGHT" lastCell="F85")</t>
         </r>
         <r>
           <rPr>
@@ -2222,7 +2247,7 @@
             <family val="2"/>
           </rPr>
           <t>Author:
-jx:each(items="sheetThree.ballastPumps[1].cargoTankUllage.status" var="ballastPumpStatus1"  direction="RIGHT" lastCell="F86")</t>
+jx:each(items="sheetThree.ballastPumps[2].cargoTankUllage.status" var="ballastPumpStatus2"  direction="RIGHT" lastCell="F86")</t>
         </r>
         <r>
           <rPr>
@@ -2376,7 +2401,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="597">
   <si>
     <t>TRIM</t>
   </si>
@@ -4133,55 +4158,67 @@
     <t>${ballastPumpStatus1.colorCode}</t>
   </si>
   <si>
-    <t>${cargoTankStatus.colorCode},${cargoTankStatus.cowType}</t>
+    <t>${cargoTankStatus.colorCode} ${cargoTankStatus.cowType}</t>
   </si>
   <si>
-    <t>${cargoTankStatus1.colorCode},${cargoTankStatus1.cowType}</t>
+    <t>${cargoTankStatus1.colorCode} ${cargoTankStatus1.cowType}</t>
   </si>
   <si>
-    <t>${cargoTankStatus2.colorCode},${cargoTankStatus2.cowType}</t>
+    <t>${cargoTankStatus2.colorCode} ${cargoTankStatus2.cowType}</t>
   </si>
   <si>
-    <t>${cargoTankStatus3.colorCode},${cargoTankStatus3.cowType}</t>
+    <t>${cargoTankStatus3.colorCode} ${cargoTankStatus3.cowType}</t>
   </si>
   <si>
-    <t>${cargoTankStatus4.colorCode},${cargoTankStatus4.cowType}</t>
+    <t>${cargoTankStatus4.colorCode} ${cargoTankStatus4.cowType}</t>
   </si>
   <si>
-    <t>${cargoTankStatus5.colorCode},${cargoTankStatus5.cowType}</t>
+    <t>${cargoTankStatus5.colorCode} ${cargoTankStatus5.cowType}</t>
   </si>
   <si>
-    <t>${cargoTankStatus6.colorCode},${cargoTankStatus6.cowType}</t>
+    <t>${cargoTankStatus6.colorCode} ${cargoTankStatus6.cowType}</t>
   </si>
   <si>
-    <t>${cargoTankStatus7.colorCode},${cargoTankStatus7.cowType}</t>
+    <t>${cargoTankStatus7.colorCode} ${cargoTankStatus7.cowType}</t>
   </si>
   <si>
-    <t>${cargoTankStatus8.colorCode},${cargoTankStatus8.cowType}</t>
+    <t>${cargoTankStatus8.colorCode} ${cargoTankStatus8.cowType}</t>
   </si>
   <si>
-    <t>${cargoTankStatus9.colorCode},${cargoTankStatus9.cowType}</t>
+    <t>${cargoTankStatus9.colorCode} ${cargoTankStatus9.cowType}</t>
   </si>
   <si>
-    <t>${cargoTankStatus10.colorCode},${cargoTankStatus10.cowType}</t>
+    <t>${cargoTankStatus10.colorCode} ${cargoTankStatus10.cowType}</t>
   </si>
   <si>
-    <t>${cargoTankStatus11.colorCode},${cargoTankStatus11.cowType}</t>
+    <t>${cargoTankStatus11.colorCode} ${cargoTankStatus11.cowType}</t>
   </si>
   <si>
-    <t>${cargoTankStatus12.colorCode},${cargoTankStatus12.cowType}</t>
+    <t>${cargoTankStatus12.colorCode} ${cargoTankStatus12.cowType}</t>
   </si>
   <si>
-    <t>${cargoTankStatus13.colorCode},${cargoTankStatus13.cowType}</t>
+    <t>${cargoTankStatus13.colorCode} ${cargoTankStatus13.cowType}</t>
   </si>
   <si>
-    <t>${cargoTankStatus14.colorCode},${cargoTankStatus14.cowType}</t>
+    <t>${cargoTankStatus14.colorCode} ${cargoTankStatus14.cowType}</t>
   </si>
   <si>
-    <t>${cargoTankStatus15.colorCode},${cargoTankStatus15.cowType}</t>
+    <t>${cargoTankStatus15.colorCode} ${cargoTankStatus15.cowType}</t>
   </si>
   <si>
-    <t>${cargoTankStatus16.colorCode},${cargoTankStatus16.cowType}</t>
+    <t>${cargoTankStatus16.colorCode} ${cargoTankStatus16.cowType}</t>
+  </si>
+  <si>
+    <t>COW TOP WASH :</t>
+  </si>
+  <si>
+    <t>COW FULL WASH :</t>
+  </si>
+  <si>
+    <t>COW BOTTOM WASH :</t>
+  </si>
+  <si>
+    <t>${ballastPumpStatus2.colorCode}</t>
   </si>
 </sst>
 </file>
@@ -5012,7 +5049,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="509">
+  <cellXfs count="511">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -5634,10 +5671,6 @@
     <xf numFmtId="0" fontId="51" fillId="0" borderId="10" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -5648,6 +5681,10 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6335,10 +6372,6 @@
       <alignment horizontal="right" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="4" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -6468,7 +6501,19 @@
     <xf numFmtId="0" fontId="37" fillId="4" borderId="18" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="4" borderId="19" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="4" borderId="15" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6480,12 +6525,6 @@
     <xf numFmtId="38" fontId="23" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="4" borderId="19" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="4" borderId="15" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6562,6 +6601,9 @@
     <xf numFmtId="0" fontId="40" fillId="3" borderId="30" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="57" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -7700,10 +7742,10 @@
           </xdr:nvGrpSpPr>
           <xdr:grpSpPr>
             <a:xfrm>
-              <a:off x="380552" y="3921604"/>
+              <a:off x="380552" y="3921619"/>
               <a:ext cx="418203" cy="725634"/>
-              <a:chOff x="376566" y="3942678"/>
-              <a:chExt cx="297180" cy="732370"/>
+              <a:chOff x="376566" y="3942676"/>
+              <a:chExt cx="297180" cy="732365"/>
             </a:xfrm>
           </xdr:grpSpPr>
           <xdr:sp macro="" textlink="">
@@ -7722,7 +7764,7 @@
             </xdr:nvSpPr>
             <xdr:spPr bwMode="auto">
               <a:xfrm>
-                <a:off x="376566" y="3942678"/>
+                <a:off x="376566" y="3942676"/>
                 <a:ext cx="297180" cy="194983"/>
               </a:xfrm>
               <a:prstGeom prst="rect">
@@ -7806,7 +7848,7 @@
             </xdr:nvSpPr>
             <xdr:spPr bwMode="auto">
               <a:xfrm>
-                <a:off x="392430" y="4404369"/>
+                <a:off x="392430" y="4404362"/>
                 <a:ext cx="243840" cy="270679"/>
               </a:xfrm>
               <a:prstGeom prst="rect">
@@ -7838,6 +7880,143 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>591678</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>133187</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>820249</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>15871</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8758525" y="21603658"/>
+          <a:ext cx="228571" cy="241270"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>333778</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>120489</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>562349</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>28570</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5891896" y="21590960"/>
+          <a:ext cx="228571" cy="266667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>219318</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>133187</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>447889</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>15871</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3105953" y="21603658"/>
+          <a:ext cx="228571" cy="241270"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8131,7 +8310,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AS73"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="17.25" customHeight="1"/>
   <cols>
@@ -11313,9 +11492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ74"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:H4"/>
-    </sheetView>
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.6640625" defaultRowHeight="17.25" customHeight="1"/>
   <cols>
@@ -11441,7 +11618,7 @@
     </row>
     <row r="4" spans="1:24" s="219" customFormat="1" ht="19.5" customHeight="1">
       <c r="A4" s="218"/>
-      <c r="B4" s="250" t="s">
+      <c r="B4" s="253" t="s">
         <v>556</v>
       </c>
       <c r="C4" s="364" t="s">
@@ -11645,13 +11822,13 @@
       <c r="H11" s="400"/>
       <c r="I11" s="400"/>
       <c r="J11" s="400"/>
-      <c r="K11" s="252" t="s">
+      <c r="K11" s="251" t="s">
         <v>484</v>
       </c>
       <c r="L11" s="233" t="s">
         <v>557</v>
       </c>
-      <c r="M11" s="251" t="s">
+      <c r="M11" s="250" t="s">
         <v>488</v>
       </c>
       <c r="O11" s="349"/>
@@ -11679,13 +11856,13 @@
       <c r="H12" s="393"/>
       <c r="I12" s="393"/>
       <c r="J12" s="393"/>
-      <c r="K12" s="253" t="s">
+      <c r="K12" s="252" t="s">
         <v>484</v>
       </c>
       <c r="L12" s="234" t="s">
         <v>558</v>
       </c>
-      <c r="M12" s="251" t="s">
+      <c r="M12" s="250" t="s">
         <v>488</v>
       </c>
       <c r="O12" s="401" t="s">
@@ -11719,13 +11896,13 @@
       <c r="H13" s="393"/>
       <c r="I13" s="393"/>
       <c r="J13" s="393"/>
-      <c r="K13" s="253" t="s">
+      <c r="K13" s="252" t="s">
         <v>484</v>
       </c>
       <c r="L13" s="234" t="s">
         <v>559</v>
       </c>
-      <c r="M13" s="251" t="s">
+      <c r="M13" s="250" t="s">
         <v>488</v>
       </c>
       <c r="O13" s="235"/>
@@ -13677,9 +13854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BW1053"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39:F39"/>
-    </sheetView>
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.33203125" defaultRowHeight="15.6"/>
   <cols>
@@ -13714,37 +13889,37 @@
       <c r="A2" s="106" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="475" t="s">
+      <c r="B2" s="478" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="475"/>
-      <c r="D2" s="475"/>
-      <c r="E2" s="486" t="s">
+      <c r="C2" s="478"/>
+      <c r="D2" s="478"/>
+      <c r="E2" s="487" t="s">
         <v>508</v>
       </c>
-      <c r="F2" s="487"/>
-      <c r="G2" s="487"/>
-      <c r="H2" s="487"/>
-      <c r="I2" s="487"/>
-      <c r="J2" s="487"/>
-      <c r="K2" s="487"/>
-      <c r="L2" s="487"/>
-      <c r="M2" s="487"/>
-      <c r="N2" s="487"/>
-      <c r="O2" s="487"/>
-      <c r="P2" s="487"/>
-      <c r="Q2" s="487"/>
-      <c r="R2" s="487"/>
-      <c r="S2" s="487"/>
-      <c r="T2" s="487"/>
-      <c r="U2" s="487"/>
-      <c r="V2" s="487"/>
-      <c r="W2" s="487"/>
-      <c r="X2" s="487"/>
-      <c r="Y2" s="487"/>
-      <c r="Z2" s="487"/>
-      <c r="AA2" s="487"/>
-      <c r="AB2" s="488"/>
+      <c r="F2" s="488"/>
+      <c r="G2" s="488"/>
+      <c r="H2" s="488"/>
+      <c r="I2" s="488"/>
+      <c r="J2" s="488"/>
+      <c r="K2" s="488"/>
+      <c r="L2" s="488"/>
+      <c r="M2" s="488"/>
+      <c r="N2" s="488"/>
+      <c r="O2" s="488"/>
+      <c r="P2" s="488"/>
+      <c r="Q2" s="488"/>
+      <c r="R2" s="488"/>
+      <c r="S2" s="488"/>
+      <c r="T2" s="488"/>
+      <c r="U2" s="488"/>
+      <c r="V2" s="488"/>
+      <c r="W2" s="488"/>
+      <c r="X2" s="488"/>
+      <c r="Y2" s="488"/>
+      <c r="Z2" s="488"/>
+      <c r="AA2" s="488"/>
+      <c r="AB2" s="489"/>
       <c r="AC2" s="107"/>
       <c r="AD2" s="107"/>
       <c r="AE2" s="107"/>
@@ -13754,54 +13929,54 @@
       <c r="AI2" s="108"/>
       <c r="AJ2" s="108"/>
       <c r="AP2" s="105"/>
-      <c r="BF2" s="476"/>
-      <c r="BG2" s="476"/>
-      <c r="BH2" s="476"/>
-      <c r="BI2" s="476"/>
-      <c r="BJ2" s="476"/>
-      <c r="BK2" s="476"/>
-      <c r="BL2" s="476"/>
-      <c r="BM2" s="476"/>
-      <c r="BN2" s="476"/>
-      <c r="BO2" s="476"/>
-      <c r="BP2" s="476"/>
-      <c r="BQ2" s="476"/>
-      <c r="BR2" s="476"/>
-      <c r="BS2" s="476"/>
+      <c r="BF2" s="479"/>
+      <c r="BG2" s="479"/>
+      <c r="BH2" s="479"/>
+      <c r="BI2" s="479"/>
+      <c r="BJ2" s="479"/>
+      <c r="BK2" s="479"/>
+      <c r="BL2" s="479"/>
+      <c r="BM2" s="479"/>
+      <c r="BN2" s="479"/>
+      <c r="BO2" s="479"/>
+      <c r="BP2" s="479"/>
+      <c r="BQ2" s="479"/>
+      <c r="BR2" s="479"/>
+      <c r="BS2" s="479"/>
     </row>
     <row r="3" spans="1:75" ht="46.8" customHeight="1" thickBot="1">
       <c r="A3" s="106" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="475" t="s">
+      <c r="B3" s="478" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="475"/>
-      <c r="D3" s="475"/>
-      <c r="E3" s="489"/>
-      <c r="F3" s="490"/>
-      <c r="G3" s="490"/>
-      <c r="H3" s="490"/>
-      <c r="I3" s="490"/>
-      <c r="J3" s="490"/>
-      <c r="K3" s="490"/>
-      <c r="L3" s="490"/>
-      <c r="M3" s="490"/>
-      <c r="N3" s="490"/>
-      <c r="O3" s="490"/>
-      <c r="P3" s="490"/>
-      <c r="Q3" s="490"/>
-      <c r="R3" s="490"/>
-      <c r="S3" s="490"/>
-      <c r="T3" s="490"/>
-      <c r="U3" s="490"/>
-      <c r="V3" s="490"/>
-      <c r="W3" s="490"/>
-      <c r="X3" s="490"/>
-      <c r="Y3" s="490"/>
-      <c r="Z3" s="490"/>
-      <c r="AA3" s="490"/>
-      <c r="AB3" s="491"/>
+      <c r="C3" s="478"/>
+      <c r="D3" s="478"/>
+      <c r="E3" s="490"/>
+      <c r="F3" s="491"/>
+      <c r="G3" s="491"/>
+      <c r="H3" s="491"/>
+      <c r="I3" s="491"/>
+      <c r="J3" s="491"/>
+      <c r="K3" s="491"/>
+      <c r="L3" s="491"/>
+      <c r="M3" s="491"/>
+      <c r="N3" s="491"/>
+      <c r="O3" s="491"/>
+      <c r="P3" s="491"/>
+      <c r="Q3" s="491"/>
+      <c r="R3" s="491"/>
+      <c r="S3" s="491"/>
+      <c r="T3" s="491"/>
+      <c r="U3" s="491"/>
+      <c r="V3" s="491"/>
+      <c r="W3" s="491"/>
+      <c r="X3" s="491"/>
+      <c r="Y3" s="491"/>
+      <c r="Z3" s="491"/>
+      <c r="AA3" s="491"/>
+      <c r="AB3" s="492"/>
       <c r="AC3" s="107"/>
       <c r="AD3" s="107"/>
       <c r="AE3" s="107"/>
@@ -13910,22 +14085,22 @@
       <c r="BO4" s="103"/>
     </row>
     <row r="5" spans="1:75" ht="18" customHeight="1">
-      <c r="A5" s="472" t="s">
+      <c r="A5" s="471" t="s">
         <v>295</v>
       </c>
-      <c r="B5" s="492" t="s">
+      <c r="B5" s="493" t="s">
         <v>388</v>
       </c>
-      <c r="C5" s="478" t="s">
+      <c r="C5" s="476" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="494" t="s">
+      <c r="D5" s="495" t="s">
         <v>389</v>
       </c>
-      <c r="E5" s="496" t="s">
+      <c r="E5" s="497" t="s">
         <v>385</v>
       </c>
-      <c r="F5" s="497"/>
+      <c r="F5" s="498"/>
       <c r="G5" s="113"/>
       <c r="H5" s="113"/>
       <c r="I5" s="113"/>
@@ -13952,10 +14127,10 @@
       <c r="AD5" s="117"/>
       <c r="AE5" s="118"/>
       <c r="AF5" s="118"/>
-      <c r="AG5" s="477"/>
-      <c r="AH5" s="477"/>
-      <c r="AI5" s="477"/>
-      <c r="AJ5" s="477"/>
+      <c r="AG5" s="480"/>
+      <c r="AH5" s="480"/>
+      <c r="AI5" s="480"/>
+      <c r="AJ5" s="480"/>
       <c r="AK5" s="119"/>
       <c r="AL5" s="120"/>
       <c r="AM5" s="121"/>
@@ -13997,12 +14172,12 @@
       <c r="BW5" s="121"/>
     </row>
     <row r="6" spans="1:75" ht="18" customHeight="1">
-      <c r="A6" s="473"/>
-      <c r="B6" s="493"/>
-      <c r="C6" s="479"/>
-      <c r="D6" s="495"/>
-      <c r="E6" s="498"/>
-      <c r="F6" s="499"/>
+      <c r="A6" s="472"/>
+      <c r="B6" s="494"/>
+      <c r="C6" s="477"/>
+      <c r="D6" s="496"/>
+      <c r="E6" s="499"/>
+      <c r="F6" s="500"/>
       <c r="G6" s="74"/>
       <c r="H6" s="74"/>
       <c r="I6" s="74"/>
@@ -14027,12 +14202,12 @@
       <c r="AB6" s="74"/>
       <c r="AC6" s="74"/>
       <c r="AD6" s="74"/>
-      <c r="AE6" s="467"/>
-      <c r="AF6" s="467"/>
+      <c r="AE6" s="466"/>
+      <c r="AF6" s="466"/>
       <c r="AG6" s="122"/>
       <c r="AH6" s="123"/>
-      <c r="AI6" s="467"/>
-      <c r="AJ6" s="467"/>
+      <c r="AI6" s="466"/>
+      <c r="AJ6" s="466"/>
       <c r="AK6" s="123"/>
       <c r="AL6" s="124"/>
       <c r="AM6" s="124"/>
@@ -14074,16 +14249,16 @@
       <c r="BW6" s="125"/>
     </row>
     <row r="7" spans="1:75">
-      <c r="A7" s="468" t="s">
+      <c r="A7" s="467" t="s">
         <v>303</v>
       </c>
-      <c r="B7" s="469" t="s">
+      <c r="B7" s="468" t="s">
         <v>304</v>
       </c>
-      <c r="C7" s="468" t="s">
+      <c r="C7" s="467" t="s">
         <v>305</v>
       </c>
-      <c r="D7" s="471" t="s">
+      <c r="D7" s="470" t="s">
         <v>306</v>
       </c>
       <c r="E7" s="435" t="s">
@@ -14139,10 +14314,10 @@
       <c r="BW7" s="132"/>
     </row>
     <row r="8" spans="1:75">
-      <c r="A8" s="468"/>
-      <c r="B8" s="470"/>
-      <c r="C8" s="468"/>
-      <c r="D8" s="471"/>
+      <c r="A8" s="467"/>
+      <c r="B8" s="469"/>
+      <c r="C8" s="467"/>
+      <c r="D8" s="470"/>
       <c r="E8" s="435" t="s">
         <v>390</v>
       </c>
@@ -14193,16 +14368,16 @@
       <c r="BW8" s="132"/>
     </row>
     <row r="9" spans="1:75" ht="15.6" customHeight="1">
-      <c r="A9" s="468" t="s">
+      <c r="A9" s="473" t="s">
         <v>307</v>
       </c>
-      <c r="B9" s="474" t="s">
+      <c r="B9" s="468" t="s">
         <v>308</v>
       </c>
-      <c r="C9" s="468" t="s">
+      <c r="C9" s="473" t="s">
         <v>309</v>
       </c>
-      <c r="D9" s="471" t="s">
+      <c r="D9" s="473" t="s">
         <v>310</v>
       </c>
       <c r="E9" s="435" t="s">
@@ -14255,10 +14430,10 @@
       <c r="BW9" s="132"/>
     </row>
     <row r="10" spans="1:75" ht="15.6" customHeight="1">
-      <c r="A10" s="468"/>
-      <c r="B10" s="474"/>
-      <c r="C10" s="468"/>
-      <c r="D10" s="471"/>
+      <c r="A10" s="474"/>
+      <c r="B10" s="469"/>
+      <c r="C10" s="474"/>
+      <c r="D10" s="474"/>
       <c r="E10" s="435" t="s">
         <v>391</v>
       </c>
@@ -14313,16 +14488,16 @@
       <c r="BW10" s="132"/>
     </row>
     <row r="11" spans="1:75" ht="15.6" customHeight="1">
-      <c r="A11" s="468" t="s">
+      <c r="A11" s="473" t="s">
         <v>311</v>
       </c>
-      <c r="B11" s="474" t="s">
+      <c r="B11" s="468" t="s">
         <v>312</v>
       </c>
-      <c r="C11" s="468" t="s">
+      <c r="C11" s="473" t="s">
         <v>313</v>
       </c>
-      <c r="D11" s="471" t="s">
+      <c r="D11" s="473" t="s">
         <v>314</v>
       </c>
       <c r="E11" s="435" t="s">
@@ -14379,11 +14554,11 @@
       <c r="BV11" s="132"/>
       <c r="BW11" s="132"/>
     </row>
-    <row r="12" spans="1:75">
-      <c r="A12" s="468"/>
-      <c r="B12" s="474"/>
-      <c r="C12" s="468"/>
-      <c r="D12" s="471"/>
+    <row r="12" spans="1:75" ht="15.6" customHeight="1">
+      <c r="A12" s="474"/>
+      <c r="B12" s="469"/>
+      <c r="C12" s="474"/>
+      <c r="D12" s="474"/>
       <c r="E12" s="435" t="s">
         <v>392</v>
       </c>
@@ -14439,16 +14614,16 @@
       <c r="BW12" s="132"/>
     </row>
     <row r="13" spans="1:75" ht="15.6" customHeight="1">
-      <c r="A13" s="468" t="s">
+      <c r="A13" s="467" t="s">
         <v>315</v>
       </c>
-      <c r="B13" s="474" t="s">
+      <c r="B13" s="475" t="s">
         <v>316</v>
       </c>
-      <c r="C13" s="468" t="s">
+      <c r="C13" s="467" t="s">
         <v>317</v>
       </c>
-      <c r="D13" s="471" t="s">
+      <c r="D13" s="470" t="s">
         <v>318</v>
       </c>
       <c r="E13" s="435" t="s">
@@ -14506,10 +14681,10 @@
       <c r="BW13" s="132"/>
     </row>
     <row r="14" spans="1:75">
-      <c r="A14" s="468"/>
-      <c r="B14" s="474"/>
-      <c r="C14" s="468"/>
-      <c r="D14" s="471"/>
+      <c r="A14" s="467"/>
+      <c r="B14" s="475"/>
+      <c r="C14" s="467"/>
+      <c r="D14" s="470"/>
       <c r="E14" s="435" t="s">
         <v>393</v>
       </c>
@@ -14565,16 +14740,16 @@
       <c r="BW14" s="132"/>
     </row>
     <row r="15" spans="1:75" ht="15.6" customHeight="1">
-      <c r="A15" s="468" t="s">
+      <c r="A15" s="473" t="s">
         <v>319</v>
       </c>
-      <c r="B15" s="474" t="s">
+      <c r="B15" s="468" t="s">
         <v>320</v>
       </c>
-      <c r="C15" s="468" t="s">
+      <c r="C15" s="473" t="s">
         <v>321</v>
       </c>
-      <c r="D15" s="471" t="s">
+      <c r="D15" s="473" t="s">
         <v>322</v>
       </c>
       <c r="E15" s="435" t="s">
@@ -14631,11 +14806,11 @@
       <c r="BV15" s="132"/>
       <c r="BW15" s="132"/>
     </row>
-    <row r="16" spans="1:75">
-      <c r="A16" s="468"/>
-      <c r="B16" s="474"/>
-      <c r="C16" s="468"/>
-      <c r="D16" s="471"/>
+    <row r="16" spans="1:75" ht="15.6" customHeight="1">
+      <c r="A16" s="474"/>
+      <c r="B16" s="469"/>
+      <c r="C16" s="474"/>
+      <c r="D16" s="474"/>
       <c r="E16" s="435" t="s">
         <v>394</v>
       </c>
@@ -14686,16 +14861,16 @@
       <c r="BW16" s="132"/>
     </row>
     <row r="17" spans="1:75" ht="15.6" customHeight="1">
-      <c r="A17" s="468" t="s">
+      <c r="A17" s="467" t="s">
         <v>323</v>
       </c>
-      <c r="B17" s="474" t="s">
+      <c r="B17" s="475" t="s">
         <v>324</v>
       </c>
-      <c r="C17" s="468" t="s">
+      <c r="C17" s="467" t="s">
         <v>325</v>
       </c>
-      <c r="D17" s="471" t="s">
+      <c r="D17" s="470" t="s">
         <v>326</v>
       </c>
       <c r="E17" s="435" t="s">
@@ -14748,10 +14923,10 @@
       <c r="BW17" s="132"/>
     </row>
     <row r="18" spans="1:75">
-      <c r="A18" s="468"/>
-      <c r="B18" s="474"/>
-      <c r="C18" s="468"/>
-      <c r="D18" s="471"/>
+      <c r="A18" s="467"/>
+      <c r="B18" s="475"/>
+      <c r="C18" s="467"/>
+      <c r="D18" s="470"/>
       <c r="E18" s="435" t="s">
         <v>395</v>
       </c>
@@ -14810,16 +14985,16 @@
       <c r="BW18" s="132"/>
     </row>
     <row r="19" spans="1:75" ht="15.6" customHeight="1">
-      <c r="A19" s="468" t="s">
+      <c r="A19" s="473" t="s">
         <v>327</v>
       </c>
-      <c r="B19" s="474" t="s">
+      <c r="B19" s="468" t="s">
         <v>328</v>
       </c>
-      <c r="C19" s="468" t="s">
+      <c r="C19" s="473" t="s">
         <v>329</v>
       </c>
-      <c r="D19" s="471" t="s">
+      <c r="D19" s="473" t="s">
         <v>330</v>
       </c>
       <c r="E19" s="435" t="s">
@@ -14871,11 +15046,11 @@
       <c r="BV19" s="132"/>
       <c r="BW19" s="132"/>
     </row>
-    <row r="20" spans="1:75">
-      <c r="A20" s="468"/>
-      <c r="B20" s="474"/>
-      <c r="C20" s="468"/>
-      <c r="D20" s="471"/>
+    <row r="20" spans="1:75" ht="15.6" customHeight="1">
+      <c r="A20" s="474"/>
+      <c r="B20" s="469"/>
+      <c r="C20" s="474"/>
+      <c r="D20" s="474"/>
       <c r="E20" s="435" t="s">
         <v>396</v>
       </c>
@@ -14926,16 +15101,16 @@
       <c r="BW20" s="132"/>
     </row>
     <row r="21" spans="1:75" ht="15.6" customHeight="1">
-      <c r="A21" s="468" t="s">
+      <c r="A21" s="467" t="s">
         <v>331</v>
       </c>
-      <c r="B21" s="474" t="s">
+      <c r="B21" s="475" t="s">
         <v>332</v>
       </c>
-      <c r="C21" s="468" t="s">
+      <c r="C21" s="467" t="s">
         <v>333</v>
       </c>
-      <c r="D21" s="471" t="s">
+      <c r="D21" s="470" t="s">
         <v>334</v>
       </c>
       <c r="E21" s="435" t="s">
@@ -14988,10 +15163,10 @@
       <c r="BW21" s="132"/>
     </row>
     <row r="22" spans="1:75">
-      <c r="A22" s="468"/>
-      <c r="B22" s="474"/>
-      <c r="C22" s="468"/>
-      <c r="D22" s="471"/>
+      <c r="A22" s="467"/>
+      <c r="B22" s="475"/>
+      <c r="C22" s="467"/>
+      <c r="D22" s="470"/>
       <c r="E22" s="435" t="s">
         <v>397</v>
       </c>
@@ -15042,16 +15217,16 @@
       <c r="BW22" s="132"/>
     </row>
     <row r="23" spans="1:75" ht="15.6" customHeight="1">
-      <c r="A23" s="468" t="s">
+      <c r="A23" s="473" t="s">
         <v>335</v>
       </c>
-      <c r="B23" s="474" t="s">
+      <c r="B23" s="468" t="s">
         <v>336</v>
       </c>
-      <c r="C23" s="468" t="s">
+      <c r="C23" s="473" t="s">
         <v>337</v>
       </c>
-      <c r="D23" s="471" t="s">
+      <c r="D23" s="473" t="s">
         <v>338</v>
       </c>
       <c r="E23" s="435" t="s">
@@ -15103,11 +15278,11 @@
       <c r="BV23" s="132"/>
       <c r="BW23" s="132"/>
     </row>
-    <row r="24" spans="1:75">
-      <c r="A24" s="468"/>
-      <c r="B24" s="474"/>
-      <c r="C24" s="468"/>
-      <c r="D24" s="471"/>
+    <row r="24" spans="1:75" ht="15.6" customHeight="1">
+      <c r="A24" s="474"/>
+      <c r="B24" s="469"/>
+      <c r="C24" s="474"/>
+      <c r="D24" s="474"/>
       <c r="E24" s="435" t="s">
         <v>398</v>
       </c>
@@ -15158,16 +15333,16 @@
       <c r="BW24" s="132"/>
     </row>
     <row r="25" spans="1:75" ht="15.6" customHeight="1">
-      <c r="A25" s="468" t="s">
+      <c r="A25" s="467" t="s">
         <v>339</v>
       </c>
-      <c r="B25" s="474" t="s">
+      <c r="B25" s="475" t="s">
         <v>340</v>
       </c>
-      <c r="C25" s="468" t="s">
+      <c r="C25" s="467" t="s">
         <v>341</v>
       </c>
-      <c r="D25" s="471" t="s">
+      <c r="D25" s="470" t="s">
         <v>342</v>
       </c>
       <c r="E25" s="435" t="s">
@@ -15220,10 +15395,10 @@
       <c r="BW25" s="132"/>
     </row>
     <row r="26" spans="1:75">
-      <c r="A26" s="468"/>
-      <c r="B26" s="474"/>
-      <c r="C26" s="468"/>
-      <c r="D26" s="471"/>
+      <c r="A26" s="467"/>
+      <c r="B26" s="475"/>
+      <c r="C26" s="467"/>
+      <c r="D26" s="470"/>
       <c r="E26" s="435" t="s">
         <v>399</v>
       </c>
@@ -15274,16 +15449,16 @@
       <c r="BW26" s="132"/>
     </row>
     <row r="27" spans="1:75" ht="15.6" customHeight="1">
-      <c r="A27" s="468" t="s">
+      <c r="A27" s="473" t="s">
         <v>343</v>
       </c>
-      <c r="B27" s="474" t="s">
+      <c r="B27" s="468" t="s">
         <v>344</v>
       </c>
-      <c r="C27" s="468" t="s">
+      <c r="C27" s="473" t="s">
         <v>345</v>
       </c>
-      <c r="D27" s="471" t="s">
+      <c r="D27" s="473" t="s">
         <v>346</v>
       </c>
       <c r="E27" s="435" t="s">
@@ -15335,11 +15510,11 @@
       <c r="BV27" s="132"/>
       <c r="BW27" s="132"/>
     </row>
-    <row r="28" spans="1:75">
-      <c r="A28" s="468"/>
-      <c r="B28" s="474"/>
-      <c r="C28" s="468"/>
-      <c r="D28" s="471"/>
+    <row r="28" spans="1:75" ht="15.6" customHeight="1">
+      <c r="A28" s="474"/>
+      <c r="B28" s="469"/>
+      <c r="C28" s="474"/>
+      <c r="D28" s="474"/>
       <c r="E28" s="435" t="s">
         <v>400</v>
       </c>
@@ -15390,16 +15565,16 @@
       <c r="BW28" s="132"/>
     </row>
     <row r="29" spans="1:75" ht="15.6" customHeight="1">
-      <c r="A29" s="468" t="s">
+      <c r="A29" s="467" t="s">
         <v>347</v>
       </c>
-      <c r="B29" s="474" t="s">
+      <c r="B29" s="475" t="s">
         <v>348</v>
       </c>
-      <c r="C29" s="468" t="s">
+      <c r="C29" s="467" t="s">
         <v>349</v>
       </c>
-      <c r="D29" s="471" t="s">
+      <c r="D29" s="470" t="s">
         <v>350</v>
       </c>
       <c r="E29" s="435" t="s">
@@ -15452,10 +15627,10 @@
       <c r="BW29" s="132"/>
     </row>
     <row r="30" spans="1:75">
-      <c r="A30" s="468"/>
-      <c r="B30" s="474"/>
-      <c r="C30" s="468"/>
-      <c r="D30" s="471"/>
+      <c r="A30" s="467"/>
+      <c r="B30" s="475"/>
+      <c r="C30" s="467"/>
+      <c r="D30" s="470"/>
       <c r="E30" s="435" t="s">
         <v>401</v>
       </c>
@@ -15506,16 +15681,16 @@
       <c r="BW30" s="132"/>
     </row>
     <row r="31" spans="1:75" ht="15.6" customHeight="1">
-      <c r="A31" s="468" t="s">
+      <c r="A31" s="467" t="s">
         <v>351</v>
       </c>
-      <c r="B31" s="474" t="s">
+      <c r="B31" s="475" t="s">
         <v>352</v>
       </c>
-      <c r="C31" s="468" t="s">
+      <c r="C31" s="467" t="s">
         <v>353</v>
       </c>
-      <c r="D31" s="471" t="s">
+      <c r="D31" s="470" t="s">
         <v>354</v>
       </c>
       <c r="E31" s="435" t="s">
@@ -15568,10 +15743,10 @@
       <c r="BW31" s="132"/>
     </row>
     <row r="32" spans="1:75">
-      <c r="A32" s="468"/>
-      <c r="B32" s="474"/>
-      <c r="C32" s="468"/>
-      <c r="D32" s="471"/>
+      <c r="A32" s="467"/>
+      <c r="B32" s="475"/>
+      <c r="C32" s="467"/>
+      <c r="D32" s="470"/>
       <c r="E32" s="435" t="s">
         <v>402</v>
       </c>
@@ -15622,16 +15797,16 @@
       <c r="BW32" s="132"/>
     </row>
     <row r="33" spans="1:75" ht="15.6" customHeight="1">
-      <c r="A33" s="468" t="s">
+      <c r="A33" s="467" t="s">
         <v>355</v>
       </c>
-      <c r="B33" s="474" t="s">
+      <c r="B33" s="475" t="s">
         <v>356</v>
       </c>
-      <c r="C33" s="468" t="s">
+      <c r="C33" s="467" t="s">
         <v>357</v>
       </c>
-      <c r="D33" s="471" t="s">
+      <c r="D33" s="470" t="s">
         <v>358</v>
       </c>
       <c r="E33" s="435" t="s">
@@ -15684,10 +15859,10 @@
       <c r="BW33" s="132"/>
     </row>
     <row r="34" spans="1:75">
-      <c r="A34" s="468"/>
-      <c r="B34" s="474"/>
-      <c r="C34" s="468"/>
-      <c r="D34" s="471"/>
+      <c r="A34" s="467"/>
+      <c r="B34" s="475"/>
+      <c r="C34" s="467"/>
+      <c r="D34" s="470"/>
       <c r="E34" s="435" t="s">
         <v>403</v>
       </c>
@@ -15738,16 +15913,16 @@
       <c r="BW34" s="132"/>
     </row>
     <row r="35" spans="1:75" ht="15.6" customHeight="1">
-      <c r="A35" s="468" t="s">
+      <c r="A35" s="467" t="s">
         <v>359</v>
       </c>
-      <c r="B35" s="474" t="s">
+      <c r="B35" s="475" t="s">
         <v>360</v>
       </c>
-      <c r="C35" s="468" t="s">
+      <c r="C35" s="467" t="s">
         <v>361</v>
       </c>
-      <c r="D35" s="471" t="s">
+      <c r="D35" s="470" t="s">
         <v>362</v>
       </c>
       <c r="E35" s="435" t="s">
@@ -15800,10 +15975,10 @@
       <c r="BW35" s="132"/>
     </row>
     <row r="36" spans="1:75">
-      <c r="A36" s="468"/>
-      <c r="B36" s="474"/>
-      <c r="C36" s="468"/>
-      <c r="D36" s="471"/>
+      <c r="A36" s="467"/>
+      <c r="B36" s="475"/>
+      <c r="C36" s="467"/>
+      <c r="D36" s="470"/>
       <c r="E36" s="435" t="s">
         <v>404</v>
       </c>
@@ -15854,16 +16029,16 @@
       <c r="BW36" s="132"/>
     </row>
     <row r="37" spans="1:75" ht="15.6" customHeight="1">
-      <c r="A37" s="468" t="s">
+      <c r="A37" s="467" t="s">
         <v>363</v>
       </c>
-      <c r="B37" s="474" t="s">
+      <c r="B37" s="475" t="s">
         <v>364</v>
       </c>
-      <c r="C37" s="468" t="s">
+      <c r="C37" s="467" t="s">
         <v>365</v>
       </c>
-      <c r="D37" s="471" t="s">
+      <c r="D37" s="470" t="s">
         <v>366</v>
       </c>
       <c r="E37" s="435" t="s">
@@ -15916,10 +16091,10 @@
       <c r="BW37" s="132"/>
     </row>
     <row r="38" spans="1:75">
-      <c r="A38" s="468"/>
-      <c r="B38" s="474"/>
-      <c r="C38" s="468"/>
-      <c r="D38" s="471"/>
+      <c r="A38" s="467"/>
+      <c r="B38" s="475"/>
+      <c r="C38" s="467"/>
+      <c r="D38" s="470"/>
       <c r="E38" s="435" t="s">
         <v>405</v>
       </c>
@@ -15970,16 +16145,16 @@
       <c r="BW38" s="132"/>
     </row>
     <row r="39" spans="1:75" ht="15.6" customHeight="1">
-      <c r="A39" s="468" t="s">
+      <c r="A39" s="467" t="s">
         <v>367</v>
       </c>
-      <c r="B39" s="474" t="s">
+      <c r="B39" s="475" t="s">
         <v>368</v>
       </c>
-      <c r="C39" s="468" t="s">
+      <c r="C39" s="467" t="s">
         <v>369</v>
       </c>
-      <c r="D39" s="471" t="s">
+      <c r="D39" s="470" t="s">
         <v>370</v>
       </c>
       <c r="E39" s="435" t="s">
@@ -16032,10 +16207,10 @@
       <c r="BW39" s="132"/>
     </row>
     <row r="40" spans="1:75">
-      <c r="A40" s="468"/>
-      <c r="B40" s="474"/>
-      <c r="C40" s="468"/>
-      <c r="D40" s="471"/>
+      <c r="A40" s="467"/>
+      <c r="B40" s="475"/>
+      <c r="C40" s="467"/>
+      <c r="D40" s="470"/>
       <c r="E40" s="435" t="s">
         <v>406</v>
       </c>
@@ -16110,18 +16285,18 @@
       <c r="BW40" s="134"/>
     </row>
     <row r="41" spans="1:75" ht="22.2" customHeight="1">
-      <c r="A41" s="482" t="s">
+      <c r="A41" s="483" t="s">
         <v>572</v>
       </c>
-      <c r="B41" s="483"/>
-      <c r="C41" s="483"/>
-      <c r="D41" s="483"/>
-      <c r="E41" s="484"/>
-      <c r="F41" s="485"/>
-      <c r="G41" s="480" t="s">
+      <c r="B41" s="484"/>
+      <c r="C41" s="484"/>
+      <c r="D41" s="484"/>
+      <c r="E41" s="485"/>
+      <c r="F41" s="486"/>
+      <c r="G41" s="481" t="s">
         <v>515</v>
       </c>
-      <c r="H41" s="481"/>
+      <c r="H41" s="482"/>
       <c r="I41" s="74"/>
       <c r="J41" s="74"/>
       <c r="K41" s="74"/>
@@ -16189,18 +16364,18 @@
       <c r="BW41" s="105"/>
     </row>
     <row r="42" spans="1:75" ht="21.6" customHeight="1">
-      <c r="A42" s="482" t="s">
+      <c r="A42" s="483" t="s">
         <v>571</v>
       </c>
-      <c r="B42" s="483"/>
-      <c r="C42" s="483"/>
-      <c r="D42" s="483"/>
-      <c r="E42" s="484"/>
-      <c r="F42" s="485"/>
-      <c r="G42" s="480" t="s">
+      <c r="B42" s="484"/>
+      <c r="C42" s="484"/>
+      <c r="D42" s="484"/>
+      <c r="E42" s="485"/>
+      <c r="F42" s="486"/>
+      <c r="G42" s="481" t="s">
         <v>565</v>
       </c>
-      <c r="H42" s="481"/>
+      <c r="H42" s="482"/>
       <c r="I42" s="74"/>
       <c r="J42" s="74"/>
       <c r="K42" s="74"/>
@@ -16268,18 +16443,18 @@
       <c r="BW42" s="105"/>
     </row>
     <row r="43" spans="1:75" ht="37.799999999999997" customHeight="1">
-      <c r="A43" s="506" t="s">
+      <c r="A43" s="508" t="s">
         <v>573</v>
       </c>
-      <c r="B43" s="507"/>
-      <c r="C43" s="507"/>
-      <c r="D43" s="507"/>
-      <c r="E43" s="507"/>
-      <c r="F43" s="508"/>
-      <c r="G43" s="502" t="s">
+      <c r="B43" s="509"/>
+      <c r="C43" s="509"/>
+      <c r="D43" s="509"/>
+      <c r="E43" s="509"/>
+      <c r="F43" s="510"/>
+      <c r="G43" s="504" t="s">
         <v>531</v>
       </c>
-      <c r="H43" s="503"/>
+      <c r="H43" s="505"/>
       <c r="I43" s="74"/>
       <c r="J43" s="74"/>
       <c r="K43" s="74"/>
@@ -16347,14 +16522,14 @@
       <c r="BW43" s="105"/>
     </row>
     <row r="44" spans="1:75">
-      <c r="A44" s="443" t="s">
+      <c r="A44" s="442" t="s">
         <v>509</v>
       </c>
-      <c r="B44" s="444"/>
-      <c r="C44" s="447" t="s">
+      <c r="B44" s="443"/>
+      <c r="C44" s="446" t="s">
         <v>510</v>
       </c>
-      <c r="D44" s="448"/>
+      <c r="D44" s="447"/>
       <c r="E44" s="435" t="s">
         <v>566</v>
       </c>
@@ -16428,10 +16603,10 @@
       <c r="BW44" s="105"/>
     </row>
     <row r="45" spans="1:75" ht="15.6" hidden="1" customHeight="1">
-      <c r="A45" s="445"/>
-      <c r="B45" s="446"/>
-      <c r="C45" s="447"/>
-      <c r="D45" s="448"/>
+      <c r="A45" s="444"/>
+      <c r="B45" s="445"/>
+      <c r="C45" s="446"/>
+      <c r="D45" s="447"/>
       <c r="E45" s="435"/>
       <c r="F45" s="436"/>
       <c r="G45" s="187"/>
@@ -16503,12 +16678,12 @@
       <c r="BW45" s="105"/>
     </row>
     <row r="46" spans="1:75">
-      <c r="A46" s="445"/>
-      <c r="B46" s="446"/>
-      <c r="C46" s="447" t="s">
+      <c r="A46" s="444"/>
+      <c r="B46" s="445"/>
+      <c r="C46" s="446" t="s">
         <v>511</v>
       </c>
-      <c r="D46" s="448"/>
+      <c r="D46" s="447"/>
       <c r="E46" s="435" t="s">
         <v>567</v>
       </c>
@@ -16582,10 +16757,10 @@
       <c r="BW46" s="105"/>
     </row>
     <row r="47" spans="1:75" ht="15.6" hidden="1" customHeight="1">
-      <c r="A47" s="445"/>
-      <c r="B47" s="446"/>
-      <c r="C47" s="447"/>
-      <c r="D47" s="448"/>
+      <c r="A47" s="444"/>
+      <c r="B47" s="445"/>
+      <c r="C47" s="446"/>
+      <c r="D47" s="447"/>
       <c r="E47" s="435"/>
       <c r="F47" s="436"/>
       <c r="G47" s="187"/>
@@ -16657,12 +16832,12 @@
       <c r="BW47" s="105"/>
     </row>
     <row r="48" spans="1:75">
-      <c r="A48" s="445"/>
-      <c r="B48" s="446"/>
-      <c r="C48" s="447" t="s">
+      <c r="A48" s="444"/>
+      <c r="B48" s="445"/>
+      <c r="C48" s="446" t="s">
         <v>512</v>
       </c>
-      <c r="D48" s="448"/>
+      <c r="D48" s="447"/>
       <c r="E48" s="435" t="s">
         <v>568</v>
       </c>
@@ -16736,10 +16911,10 @@
       <c r="BW48" s="105"/>
     </row>
     <row r="49" spans="1:75" ht="15.6" hidden="1" customHeight="1">
-      <c r="A49" s="445"/>
-      <c r="B49" s="446"/>
-      <c r="C49" s="447"/>
-      <c r="D49" s="448"/>
+      <c r="A49" s="444"/>
+      <c r="B49" s="445"/>
+      <c r="C49" s="446"/>
+      <c r="D49" s="447"/>
       <c r="E49" s="435"/>
       <c r="F49" s="436"/>
       <c r="G49" s="187"/>
@@ -16811,12 +16986,12 @@
       <c r="BW49" s="105"/>
     </row>
     <row r="50" spans="1:75">
-      <c r="A50" s="445"/>
-      <c r="B50" s="446"/>
-      <c r="C50" s="447" t="s">
+      <c r="A50" s="444"/>
+      <c r="B50" s="445"/>
+      <c r="C50" s="446" t="s">
         <v>513</v>
       </c>
-      <c r="D50" s="448"/>
+      <c r="D50" s="447"/>
       <c r="E50" s="435" t="s">
         <v>569</v>
       </c>
@@ -16890,10 +17065,10 @@
       <c r="BW50" s="105"/>
     </row>
     <row r="51" spans="1:75" ht="15.6" hidden="1" customHeight="1">
-      <c r="A51" s="445"/>
-      <c r="B51" s="446"/>
-      <c r="C51" s="447"/>
-      <c r="D51" s="448"/>
+      <c r="A51" s="444"/>
+      <c r="B51" s="445"/>
+      <c r="C51" s="446"/>
+      <c r="D51" s="447"/>
       <c r="E51" s="435"/>
       <c r="F51" s="436"/>
       <c r="G51" s="187"/>
@@ -16965,12 +17140,12 @@
       <c r="BW51" s="105"/>
     </row>
     <row r="52" spans="1:75">
-      <c r="A52" s="445"/>
-      <c r="B52" s="446"/>
-      <c r="C52" s="447" t="s">
+      <c r="A52" s="444"/>
+      <c r="B52" s="445"/>
+      <c r="C52" s="446" t="s">
         <v>514</v>
       </c>
-      <c r="D52" s="448"/>
+      <c r="D52" s="447"/>
       <c r="E52" s="435" t="s">
         <v>570</v>
       </c>
@@ -17044,10 +17219,10 @@
       <c r="BW52" s="105"/>
     </row>
     <row r="53" spans="1:75" ht="15.6" hidden="1" customHeight="1">
-      <c r="A53" s="504"/>
-      <c r="B53" s="505"/>
-      <c r="C53" s="500"/>
-      <c r="D53" s="501"/>
+      <c r="A53" s="506"/>
+      <c r="B53" s="507"/>
+      <c r="C53" s="502"/>
+      <c r="D53" s="503"/>
       <c r="E53" s="435"/>
       <c r="F53" s="436"/>
       <c r="G53" s="187"/>
@@ -17119,10 +17294,10 @@
       <c r="BW53" s="105"/>
     </row>
     <row r="54" spans="1:75" s="136" customFormat="1" ht="15" customHeight="1">
-      <c r="A54" s="449" t="s">
+      <c r="A54" s="448" t="s">
         <v>302</v>
       </c>
-      <c r="B54" s="450"/>
+      <c r="B54" s="449"/>
       <c r="C54" s="431" t="s">
         <v>371</v>
       </c>
@@ -17200,8 +17375,8 @@
       <c r="BW54" s="137"/>
     </row>
     <row r="55" spans="1:75" s="136" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A55" s="451"/>
-      <c r="B55" s="452"/>
+      <c r="A55" s="450"/>
+      <c r="B55" s="451"/>
       <c r="C55" s="433"/>
       <c r="D55" s="434"/>
       <c r="E55" s="435" t="s">
@@ -17277,8 +17452,8 @@
       <c r="BW55" s="137"/>
     </row>
     <row r="56" spans="1:75" s="136" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A56" s="451"/>
-      <c r="B56" s="452"/>
+      <c r="A56" s="450"/>
+      <c r="B56" s="451"/>
       <c r="C56" s="431" t="s">
         <v>372</v>
       </c>
@@ -17356,8 +17531,8 @@
       <c r="BW56" s="137"/>
     </row>
     <row r="57" spans="1:75" s="136" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A57" s="451"/>
-      <c r="B57" s="452"/>
+      <c r="A57" s="450"/>
+      <c r="B57" s="451"/>
       <c r="C57" s="433"/>
       <c r="D57" s="434"/>
       <c r="E57" s="435" t="s">
@@ -17433,8 +17608,8 @@
       <c r="BW57" s="137"/>
     </row>
     <row r="58" spans="1:75" s="136" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A58" s="451"/>
-      <c r="B58" s="452"/>
+      <c r="A58" s="450"/>
+      <c r="B58" s="451"/>
       <c r="C58" s="431" t="s">
         <v>373</v>
       </c>
@@ -17467,10 +17642,10 @@
       <c r="AD58" s="74"/>
       <c r="AE58" s="74"/>
       <c r="AF58" s="74"/>
-      <c r="AG58" s="456"/>
-      <c r="AH58" s="456"/>
-      <c r="AI58" s="456"/>
-      <c r="AJ58" s="456"/>
+      <c r="AG58" s="455"/>
+      <c r="AH58" s="455"/>
+      <c r="AI58" s="455"/>
+      <c r="AJ58" s="455"/>
       <c r="AK58" s="137"/>
       <c r="AL58" s="137"/>
       <c r="AM58" s="137"/>
@@ -17512,8 +17687,8 @@
       <c r="BW58" s="137"/>
     </row>
     <row r="59" spans="1:75" s="136" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A59" s="451"/>
-      <c r="B59" s="452"/>
+      <c r="A59" s="450"/>
+      <c r="B59" s="451"/>
       <c r="C59" s="433"/>
       <c r="D59" s="434"/>
       <c r="E59" s="435" t="s">
@@ -17589,8 +17764,8 @@
       <c r="BW59" s="137"/>
     </row>
     <row r="60" spans="1:75" s="136" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A60" s="451"/>
-      <c r="B60" s="452"/>
+      <c r="A60" s="450"/>
+      <c r="B60" s="451"/>
       <c r="C60" s="431" t="s">
         <v>374</v>
       </c>
@@ -17623,10 +17798,10 @@
       <c r="AD60" s="74"/>
       <c r="AE60" s="74"/>
       <c r="AF60" s="74"/>
-      <c r="AG60" s="456"/>
-      <c r="AH60" s="456"/>
-      <c r="AI60" s="456"/>
-      <c r="AJ60" s="456"/>
+      <c r="AG60" s="455"/>
+      <c r="AH60" s="455"/>
+      <c r="AI60" s="455"/>
+      <c r="AJ60" s="455"/>
       <c r="AK60" s="137"/>
       <c r="AL60" s="137"/>
       <c r="AM60" s="137"/>
@@ -17668,8 +17843,8 @@
       <c r="BW60" s="137"/>
     </row>
     <row r="61" spans="1:75" s="136" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A61" s="451"/>
-      <c r="B61" s="452"/>
+      <c r="A61" s="450"/>
+      <c r="B61" s="451"/>
       <c r="C61" s="433"/>
       <c r="D61" s="434"/>
       <c r="E61" s="435" t="s">
@@ -17745,8 +17920,8 @@
       <c r="BW61" s="137"/>
     </row>
     <row r="62" spans="1:75" s="136" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A62" s="451"/>
-      <c r="B62" s="452"/>
+      <c r="A62" s="450"/>
+      <c r="B62" s="451"/>
       <c r="C62" s="431" t="s">
         <v>375</v>
       </c>
@@ -17779,10 +17954,10 @@
       <c r="AD62" s="74"/>
       <c r="AE62" s="74"/>
       <c r="AF62" s="74"/>
-      <c r="AG62" s="456"/>
-      <c r="AH62" s="456"/>
-      <c r="AI62" s="456"/>
-      <c r="AJ62" s="456"/>
+      <c r="AG62" s="455"/>
+      <c r="AH62" s="455"/>
+      <c r="AI62" s="455"/>
+      <c r="AJ62" s="455"/>
       <c r="AK62" s="137"/>
       <c r="AL62" s="137"/>
       <c r="AM62" s="137"/>
@@ -17824,8 +17999,8 @@
       <c r="BW62" s="137"/>
     </row>
     <row r="63" spans="1:75" s="136" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A63" s="451"/>
-      <c r="B63" s="452"/>
+      <c r="A63" s="450"/>
+      <c r="B63" s="451"/>
       <c r="C63" s="433"/>
       <c r="D63" s="434"/>
       <c r="E63" s="435" t="s">
@@ -17901,8 +18076,8 @@
       <c r="BW63" s="137"/>
     </row>
     <row r="64" spans="1:75" s="136" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A64" s="451"/>
-      <c r="B64" s="452"/>
+      <c r="A64" s="450"/>
+      <c r="B64" s="451"/>
       <c r="C64" s="431" t="s">
         <v>376</v>
       </c>
@@ -17935,10 +18110,10 @@
       <c r="AD64" s="74"/>
       <c r="AE64" s="74"/>
       <c r="AF64" s="74"/>
-      <c r="AG64" s="456"/>
-      <c r="AH64" s="456"/>
-      <c r="AI64" s="456"/>
-      <c r="AJ64" s="456"/>
+      <c r="AG64" s="455"/>
+      <c r="AH64" s="455"/>
+      <c r="AI64" s="455"/>
+      <c r="AJ64" s="455"/>
       <c r="AK64" s="137"/>
       <c r="AL64" s="137"/>
       <c r="AM64" s="137"/>
@@ -17980,8 +18155,8 @@
       <c r="BW64" s="137"/>
     </row>
     <row r="65" spans="1:75" s="136" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A65" s="451"/>
-      <c r="B65" s="452"/>
+      <c r="A65" s="450"/>
+      <c r="B65" s="451"/>
       <c r="C65" s="433"/>
       <c r="D65" s="434"/>
       <c r="E65" s="435" t="s">
@@ -18057,8 +18232,8 @@
       <c r="BW65" s="137"/>
     </row>
     <row r="66" spans="1:75" s="136" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A66" s="451"/>
-      <c r="B66" s="452"/>
+      <c r="A66" s="450"/>
+      <c r="B66" s="451"/>
       <c r="C66" s="431" t="s">
         <v>377</v>
       </c>
@@ -18091,10 +18266,10 @@
       <c r="AD66" s="74"/>
       <c r="AE66" s="74"/>
       <c r="AF66" s="74"/>
-      <c r="AG66" s="456"/>
-      <c r="AH66" s="456"/>
-      <c r="AI66" s="456"/>
-      <c r="AJ66" s="456"/>
+      <c r="AG66" s="455"/>
+      <c r="AH66" s="455"/>
+      <c r="AI66" s="455"/>
+      <c r="AJ66" s="455"/>
       <c r="AK66" s="137"/>
       <c r="AL66" s="137"/>
       <c r="AM66" s="137"/>
@@ -18136,8 +18311,8 @@
       <c r="BW66" s="137"/>
     </row>
     <row r="67" spans="1:75" s="136" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A67" s="451"/>
-      <c r="B67" s="452"/>
+      <c r="A67" s="450"/>
+      <c r="B67" s="451"/>
       <c r="C67" s="433"/>
       <c r="D67" s="434"/>
       <c r="E67" s="435" t="s">
@@ -18213,8 +18388,8 @@
       <c r="BW67" s="137"/>
     </row>
     <row r="68" spans="1:75" s="136" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A68" s="451"/>
-      <c r="B68" s="452"/>
+      <c r="A68" s="450"/>
+      <c r="B68" s="451"/>
       <c r="C68" s="431" t="s">
         <v>378</v>
       </c>
@@ -18247,10 +18422,10 @@
       <c r="AD68" s="74"/>
       <c r="AE68" s="74"/>
       <c r="AF68" s="74"/>
-      <c r="AG68" s="456"/>
-      <c r="AH68" s="456"/>
-      <c r="AI68" s="456"/>
-      <c r="AJ68" s="456"/>
+      <c r="AG68" s="455"/>
+      <c r="AH68" s="455"/>
+      <c r="AI68" s="455"/>
+      <c r="AJ68" s="455"/>
       <c r="AK68" s="137"/>
       <c r="AL68" s="137"/>
       <c r="AM68" s="137"/>
@@ -18292,8 +18467,8 @@
       <c r="BW68" s="137"/>
     </row>
     <row r="69" spans="1:75" s="136" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A69" s="451"/>
-      <c r="B69" s="452"/>
+      <c r="A69" s="450"/>
+      <c r="B69" s="451"/>
       <c r="C69" s="433"/>
       <c r="D69" s="434"/>
       <c r="E69" s="435" t="s">
@@ -18369,8 +18544,8 @@
       <c r="BW69" s="137"/>
     </row>
     <row r="70" spans="1:75" s="136" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A70" s="451"/>
-      <c r="B70" s="452"/>
+      <c r="A70" s="450"/>
+      <c r="B70" s="451"/>
       <c r="C70" s="431" t="s">
         <v>379</v>
       </c>
@@ -18403,10 +18578,10 @@
       <c r="AD70" s="74"/>
       <c r="AE70" s="74"/>
       <c r="AF70" s="74"/>
-      <c r="AG70" s="456"/>
-      <c r="AH70" s="456"/>
-      <c r="AI70" s="456"/>
-      <c r="AJ70" s="456"/>
+      <c r="AG70" s="455"/>
+      <c r="AH70" s="455"/>
+      <c r="AI70" s="455"/>
+      <c r="AJ70" s="455"/>
       <c r="AK70" s="137"/>
       <c r="AL70" s="139"/>
       <c r="AM70" s="137"/>
@@ -18448,8 +18623,8 @@
       <c r="BW70" s="137"/>
     </row>
     <row r="71" spans="1:75" s="136" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A71" s="451"/>
-      <c r="B71" s="452"/>
+      <c r="A71" s="450"/>
+      <c r="B71" s="451"/>
       <c r="C71" s="433"/>
       <c r="D71" s="434"/>
       <c r="E71" s="435" t="s">
@@ -18525,8 +18700,8 @@
       <c r="BW71" s="137"/>
     </row>
     <row r="72" spans="1:75" s="136" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A72" s="451"/>
-      <c r="B72" s="452"/>
+      <c r="A72" s="450"/>
+      <c r="B72" s="451"/>
       <c r="C72" s="431" t="s">
         <v>380</v>
       </c>
@@ -18559,10 +18734,10 @@
       <c r="AD72" s="74"/>
       <c r="AE72" s="74"/>
       <c r="AF72" s="74"/>
-      <c r="AG72" s="456"/>
-      <c r="AH72" s="456"/>
-      <c r="AI72" s="456"/>
-      <c r="AJ72" s="456"/>
+      <c r="AG72" s="455"/>
+      <c r="AH72" s="455"/>
+      <c r="AI72" s="455"/>
+      <c r="AJ72" s="455"/>
       <c r="AK72" s="137"/>
       <c r="AL72" s="138"/>
       <c r="AM72" s="137"/>
@@ -18604,8 +18779,8 @@
       <c r="BW72" s="137"/>
     </row>
     <row r="73" spans="1:75" s="136" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A73" s="451"/>
-      <c r="B73" s="452"/>
+      <c r="A73" s="450"/>
+      <c r="B73" s="451"/>
       <c r="C73" s="433"/>
       <c r="D73" s="434"/>
       <c r="E73" s="435" t="s">
@@ -18681,8 +18856,8 @@
       <c r="BW73" s="137"/>
     </row>
     <row r="74" spans="1:75" s="136" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A74" s="451"/>
-      <c r="B74" s="452"/>
+      <c r="A74" s="450"/>
+      <c r="B74" s="451"/>
       <c r="C74" s="431" t="s">
         <v>381</v>
       </c>
@@ -18715,10 +18890,10 @@
       <c r="AD74" s="74"/>
       <c r="AE74" s="74"/>
       <c r="AF74" s="74"/>
-      <c r="AG74" s="456"/>
-      <c r="AH74" s="456"/>
-      <c r="AI74" s="456"/>
-      <c r="AJ74" s="456"/>
+      <c r="AG74" s="455"/>
+      <c r="AH74" s="455"/>
+      <c r="AI74" s="455"/>
+      <c r="AJ74" s="455"/>
       <c r="AK74" s="143"/>
       <c r="AL74" s="139"/>
       <c r="AM74" s="137"/>
@@ -18760,8 +18935,8 @@
       <c r="BW74" s="137"/>
     </row>
     <row r="75" spans="1:75" s="136" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A75" s="451"/>
-      <c r="B75" s="452"/>
+      <c r="A75" s="450"/>
+      <c r="B75" s="451"/>
       <c r="C75" s="433"/>
       <c r="D75" s="434"/>
       <c r="E75" s="435" t="s">
@@ -18837,8 +19012,8 @@
       <c r="BW75" s="137"/>
     </row>
     <row r="76" spans="1:75" s="136" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A76" s="451"/>
-      <c r="B76" s="452"/>
+      <c r="A76" s="450"/>
+      <c r="B76" s="451"/>
       <c r="C76" s="431" t="s">
         <v>382</v>
       </c>
@@ -18871,10 +19046,10 @@
       <c r="AD76" s="74"/>
       <c r="AE76" s="74"/>
       <c r="AF76" s="74"/>
-      <c r="AG76" s="456"/>
-      <c r="AH76" s="456"/>
-      <c r="AI76" s="456"/>
-      <c r="AJ76" s="456"/>
+      <c r="AG76" s="455"/>
+      <c r="AH76" s="455"/>
+      <c r="AI76" s="455"/>
+      <c r="AJ76" s="455"/>
       <c r="AK76" s="137"/>
       <c r="AL76" s="138"/>
       <c r="AM76" s="137"/>
@@ -18916,8 +19091,8 @@
       <c r="BW76" s="137"/>
     </row>
     <row r="77" spans="1:75" s="136" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A77" s="451"/>
-      <c r="B77" s="452"/>
+      <c r="A77" s="450"/>
+      <c r="B77" s="451"/>
       <c r="C77" s="433"/>
       <c r="D77" s="434"/>
       <c r="E77" s="435" t="s">
@@ -18993,8 +19168,8 @@
       <c r="BW77" s="137"/>
     </row>
     <row r="78" spans="1:75" s="136" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A78" s="451"/>
-      <c r="B78" s="452"/>
+      <c r="A78" s="450"/>
+      <c r="B78" s="451"/>
       <c r="C78" s="431" t="s">
         <v>383</v>
       </c>
@@ -19027,10 +19202,10 @@
       <c r="AD78" s="74"/>
       <c r="AE78" s="74"/>
       <c r="AF78" s="74"/>
-      <c r="AG78" s="456"/>
-      <c r="AH78" s="456"/>
-      <c r="AI78" s="456"/>
-      <c r="AJ78" s="456"/>
+      <c r="AG78" s="455"/>
+      <c r="AH78" s="455"/>
+      <c r="AI78" s="455"/>
+      <c r="AJ78" s="455"/>
       <c r="AK78" s="143"/>
       <c r="AL78" s="139"/>
       <c r="AM78" s="137"/>
@@ -19072,8 +19247,8 @@
       <c r="BW78" s="137"/>
     </row>
     <row r="79" spans="1:75" s="136" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A79" s="451"/>
-      <c r="B79" s="452"/>
+      <c r="A79" s="450"/>
+      <c r="B79" s="451"/>
       <c r="C79" s="433"/>
       <c r="D79" s="434"/>
       <c r="E79" s="435" t="s">
@@ -19149,8 +19324,8 @@
       <c r="BW79" s="137"/>
     </row>
     <row r="80" spans="1:75" s="136" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A80" s="451"/>
-      <c r="B80" s="452"/>
+      <c r="A80" s="450"/>
+      <c r="B80" s="451"/>
       <c r="C80" s="431" t="s">
         <v>384</v>
       </c>
@@ -19185,10 +19360,10 @@
       <c r="AD80" s="74"/>
       <c r="AE80" s="74"/>
       <c r="AF80" s="74"/>
-      <c r="AG80" s="456"/>
-      <c r="AH80" s="456"/>
-      <c r="AI80" s="456"/>
-      <c r="AJ80" s="456"/>
+      <c r="AG80" s="455"/>
+      <c r="AH80" s="455"/>
+      <c r="AI80" s="455"/>
+      <c r="AJ80" s="455"/>
       <c r="AK80" s="138"/>
       <c r="AL80" s="138"/>
       <c r="AM80" s="137"/>
@@ -19230,8 +19405,8 @@
       <c r="BW80" s="137"/>
     </row>
     <row r="81" spans="1:75" s="136" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A81" s="451"/>
-      <c r="B81" s="452"/>
+      <c r="A81" s="450"/>
+      <c r="B81" s="451"/>
       <c r="C81" s="433"/>
       <c r="D81" s="434"/>
       <c r="E81" s="435" t="s">
@@ -19309,8 +19484,8 @@
       <c r="BW81" s="137"/>
     </row>
     <row r="82" spans="1:75" s="136" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A82" s="451"/>
-      <c r="B82" s="452"/>
+      <c r="A82" s="450"/>
+      <c r="B82" s="451"/>
       <c r="C82" s="431" t="s">
         <v>386</v>
       </c>
@@ -19390,8 +19565,8 @@
       <c r="BW82" s="137"/>
     </row>
     <row r="83" spans="1:75" s="136" customFormat="1" ht="15.6" customHeight="1">
-      <c r="A83" s="451"/>
-      <c r="B83" s="452"/>
+      <c r="A83" s="450"/>
+      <c r="B83" s="451"/>
       <c r="C83" s="433"/>
       <c r="D83" s="434"/>
       <c r="E83" s="435" t="s">
@@ -19471,12 +19646,14 @@
     <row r="84" spans="1:75" s="136" customFormat="1" ht="18">
       <c r="A84" s="184"/>
       <c r="B84" s="185"/>
-      <c r="C84" s="447" t="s">
+      <c r="C84" s="446" t="s">
         <v>31</v>
       </c>
-      <c r="D84" s="448"/>
-      <c r="E84" s="437"/>
-      <c r="F84" s="436"/>
+      <c r="D84" s="447"/>
+      <c r="E84" s="437" t="s">
+        <v>574</v>
+      </c>
+      <c r="F84" s="438"/>
       <c r="G84" s="74"/>
       <c r="H84"/>
       <c r="I84"/>
@@ -19550,14 +19727,14 @@
     <row r="85" spans="1:75" s="136" customFormat="1" ht="18">
       <c r="A85" s="184"/>
       <c r="B85" s="185"/>
-      <c r="C85" s="447" t="s">
+      <c r="C85" s="446" t="s">
         <v>3</v>
       </c>
-      <c r="D85" s="448"/>
-      <c r="E85" s="438" t="s">
-        <v>574</v>
+      <c r="D85" s="447"/>
+      <c r="E85" s="437" t="s">
+        <v>575</v>
       </c>
-      <c r="F85" s="439"/>
+      <c r="F85" s="438"/>
       <c r="G85" s="74"/>
       <c r="H85"/>
       <c r="I85"/>
@@ -19631,14 +19808,14 @@
     <row r="86" spans="1:75" s="136" customFormat="1" ht="18">
       <c r="A86" s="184"/>
       <c r="B86" s="185"/>
-      <c r="C86" s="447" t="s">
+      <c r="C86" s="446" t="s">
         <v>4</v>
       </c>
-      <c r="D86" s="448"/>
-      <c r="E86" s="438" t="s">
-        <v>575</v>
+      <c r="D86" s="447"/>
+      <c r="E86" s="437" t="s">
+        <v>596</v>
       </c>
-      <c r="F86" s="439"/>
+      <c r="F86" s="438"/>
       <c r="G86" s="74"/>
       <c r="H86"/>
       <c r="I86"/>
@@ -19710,14 +19887,14 @@
       <c r="BW86" s="137"/>
     </row>
     <row r="87" spans="1:75" s="136" customFormat="1" ht="27" customHeight="1">
-      <c r="A87" s="443" t="s">
+      <c r="A87" s="442" t="s">
         <v>1</v>
       </c>
-      <c r="B87" s="444"/>
-      <c r="C87" s="441" t="s">
+      <c r="B87" s="443"/>
+      <c r="C87" s="440" t="s">
         <v>5</v>
       </c>
-      <c r="D87" s="442"/>
+      <c r="D87" s="441"/>
       <c r="E87" s="435" t="s">
         <v>296</v>
       </c>
@@ -19748,10 +19925,10 @@
       <c r="AD87" s="74"/>
       <c r="AE87" s="74"/>
       <c r="AF87" s="74"/>
-      <c r="AG87" s="454"/>
-      <c r="AH87" s="454"/>
-      <c r="AI87" s="454"/>
-      <c r="AJ87" s="454"/>
+      <c r="AG87" s="453"/>
+      <c r="AH87" s="453"/>
+      <c r="AI87" s="453"/>
+      <c r="AJ87" s="453"/>
       <c r="AK87" s="143"/>
       <c r="AL87" s="137"/>
       <c r="AM87" s="137"/>
@@ -19793,12 +19970,12 @@
       <c r="BW87" s="137"/>
     </row>
     <row r="88" spans="1:75" s="136" customFormat="1" ht="27" customHeight="1">
-      <c r="A88" s="445"/>
-      <c r="B88" s="446"/>
-      <c r="C88" s="441" t="s">
+      <c r="A88" s="444"/>
+      <c r="B88" s="445"/>
+      <c r="C88" s="440" t="s">
         <v>6</v>
       </c>
-      <c r="D88" s="442"/>
+      <c r="D88" s="441"/>
       <c r="E88" s="435" t="s">
         <v>297</v>
       </c>
@@ -19829,10 +20006,10 @@
       <c r="AD88" s="74"/>
       <c r="AE88" s="74"/>
       <c r="AF88" s="74"/>
-      <c r="AG88" s="454"/>
-      <c r="AH88" s="454"/>
-      <c r="AI88" s="454"/>
-      <c r="AJ88" s="454"/>
+      <c r="AG88" s="453"/>
+      <c r="AH88" s="453"/>
+      <c r="AI88" s="453"/>
+      <c r="AJ88" s="453"/>
       <c r="AK88" s="143"/>
       <c r="AL88" s="137"/>
       <c r="AM88" s="137"/>
@@ -19874,12 +20051,12 @@
       <c r="BW88" s="137"/>
     </row>
     <row r="89" spans="1:75" s="136" customFormat="1" ht="27" customHeight="1">
-      <c r="A89" s="445"/>
-      <c r="B89" s="446"/>
-      <c r="C89" s="441" t="s">
+      <c r="A89" s="444"/>
+      <c r="B89" s="445"/>
+      <c r="C89" s="440" t="s">
         <v>0</v>
       </c>
-      <c r="D89" s="442"/>
+      <c r="D89" s="441"/>
       <c r="E89" s="435" t="s">
         <v>298</v>
       </c>
@@ -19910,10 +20087,10 @@
       <c r="AD89" s="74"/>
       <c r="AE89" s="74"/>
       <c r="AF89" s="74"/>
-      <c r="AG89" s="455"/>
-      <c r="AH89" s="455"/>
-      <c r="AI89" s="455"/>
-      <c r="AJ89" s="455"/>
+      <c r="AG89" s="454"/>
+      <c r="AH89" s="454"/>
+      <c r="AI89" s="454"/>
+      <c r="AJ89" s="454"/>
       <c r="AK89" s="143"/>
       <c r="AL89" s="137"/>
       <c r="AM89" s="137"/>
@@ -19955,12 +20132,12 @@
       <c r="BW89" s="137"/>
     </row>
     <row r="90" spans="1:75" s="136" customFormat="1" ht="27" customHeight="1">
-      <c r="A90" s="445"/>
-      <c r="B90" s="446"/>
-      <c r="C90" s="441" t="s">
+      <c r="A90" s="444"/>
+      <c r="B90" s="445"/>
+      <c r="C90" s="440" t="s">
         <v>48</v>
       </c>
-      <c r="D90" s="442"/>
+      <c r="D90" s="441"/>
       <c r="E90" s="435" t="s">
         <v>299</v>
       </c>
@@ -20036,12 +20213,12 @@
       <c r="BW90" s="137"/>
     </row>
     <row r="91" spans="1:75" s="136" customFormat="1" ht="27" customHeight="1">
-      <c r="A91" s="445"/>
-      <c r="B91" s="446"/>
-      <c r="C91" s="441" t="s">
+      <c r="A91" s="444"/>
+      <c r="B91" s="445"/>
+      <c r="C91" s="440" t="s">
         <v>34</v>
       </c>
-      <c r="D91" s="442"/>
+      <c r="D91" s="441"/>
       <c r="E91" s="435" t="s">
         <v>387</v>
       </c>
@@ -20072,10 +20249,10 @@
       <c r="AD91" s="74"/>
       <c r="AE91" s="74"/>
       <c r="AF91" s="74"/>
-      <c r="AG91" s="455"/>
-      <c r="AH91" s="455"/>
-      <c r="AI91" s="455"/>
-      <c r="AJ91" s="455"/>
+      <c r="AG91" s="454"/>
+      <c r="AH91" s="454"/>
+      <c r="AI91" s="454"/>
+      <c r="AJ91" s="454"/>
       <c r="AK91" s="143"/>
       <c r="AL91" s="137"/>
       <c r="AM91" s="137"/>
@@ -20117,12 +20294,12 @@
       <c r="BW91" s="137"/>
     </row>
     <row r="92" spans="1:75" s="136" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A92" s="440" t="s">
+      <c r="A92" s="439" t="s">
         <v>44</v>
       </c>
-      <c r="B92" s="440"/>
-      <c r="C92" s="440"/>
-      <c r="D92" s="440"/>
+      <c r="B92" s="439"/>
+      <c r="C92" s="439"/>
+      <c r="D92" s="439"/>
       <c r="E92" s="435" t="s">
         <v>300</v>
       </c>
@@ -20153,10 +20330,10 @@
       <c r="AD92" s="74"/>
       <c r="AE92" s="74"/>
       <c r="AF92" s="74"/>
-      <c r="AG92" s="453"/>
-      <c r="AH92" s="453"/>
-      <c r="AI92" s="453"/>
-      <c r="AJ92" s="453"/>
+      <c r="AG92" s="452"/>
+      <c r="AH92" s="452"/>
+      <c r="AI92" s="452"/>
+      <c r="AJ92" s="452"/>
       <c r="AK92" s="143"/>
       <c r="AL92" s="137"/>
       <c r="AM92" s="137"/>
@@ -20198,12 +20375,12 @@
       <c r="BW92" s="137"/>
     </row>
     <row r="93" spans="1:75" s="136" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A93" s="440" t="s">
+      <c r="A93" s="439" t="s">
         <v>45</v>
       </c>
-      <c r="B93" s="440"/>
-      <c r="C93" s="440"/>
-      <c r="D93" s="440"/>
+      <c r="B93" s="439"/>
+      <c r="C93" s="439"/>
+      <c r="D93" s="439"/>
       <c r="E93" s="435" t="s">
         <v>301</v>
       </c>
@@ -20234,10 +20411,10 @@
       <c r="AD93" s="74"/>
       <c r="AE93" s="74"/>
       <c r="AF93" s="74"/>
-      <c r="AG93" s="453"/>
-      <c r="AH93" s="453"/>
-      <c r="AI93" s="453"/>
-      <c r="AJ93" s="453"/>
+      <c r="AG93" s="452"/>
+      <c r="AH93" s="452"/>
+      <c r="AI93" s="452"/>
+      <c r="AJ93" s="452"/>
       <c r="AK93" s="143"/>
       <c r="AL93" s="137"/>
       <c r="AM93" s="137"/>
@@ -20285,17 +20462,17 @@
       <c r="D94" s="146"/>
       <c r="E94" s="146"/>
       <c r="F94" s="146"/>
-      <c r="G94" s="457"/>
-      <c r="H94" s="457"/>
-      <c r="I94" s="457"/>
+      <c r="G94" s="456"/>
+      <c r="H94" s="456"/>
+      <c r="I94" s="456"/>
       <c r="J94" s="146"/>
       <c r="K94" s="146"/>
       <c r="L94" s="146"/>
       <c r="M94" s="146"/>
       <c r="N94" s="146"/>
-      <c r="O94" s="457"/>
-      <c r="P94" s="457"/>
-      <c r="Q94" s="457"/>
+      <c r="O94" s="456"/>
+      <c r="P94" s="456"/>
+      <c r="Q94" s="456"/>
       <c r="R94" s="146"/>
       <c r="S94" s="146"/>
       <c r="T94" s="146"/>
@@ -20324,10 +20501,10 @@
         <v>438</v>
       </c>
       <c r="C95" s="153"/>
-      <c r="D95" s="466" t="s">
+      <c r="D95" s="465" t="s">
         <v>54</v>
       </c>
-      <c r="E95" s="466"/>
+      <c r="E95" s="465"/>
       <c r="F95" s="146"/>
       <c r="G95" s="152"/>
       <c r="H95" s="152"/>
@@ -20368,10 +20545,10 @@
         <v>439</v>
       </c>
       <c r="C96" s="153"/>
-      <c r="D96" s="466" t="s">
+      <c r="D96" s="465" t="s">
         <v>55</v>
       </c>
-      <c r="E96" s="466"/>
+      <c r="E96" s="465"/>
       <c r="F96" s="146"/>
       <c r="G96" s="152"/>
       <c r="H96" s="152"/>
@@ -20413,9 +20590,9 @@
       <c r="D97" s="146"/>
       <c r="E97" s="146"/>
       <c r="F97" s="146"/>
-      <c r="G97" s="459"/>
-      <c r="H97" s="459"/>
-      <c r="I97" s="459"/>
+      <c r="G97" s="458"/>
+      <c r="H97" s="458"/>
+      <c r="I97" s="458"/>
       <c r="J97" s="146"/>
       <c r="K97" s="146"/>
       <c r="L97" s="146"/>
@@ -20448,35 +20625,35 @@
     </row>
     <row r="98" spans="1:75" ht="14.1" customHeight="1">
       <c r="A98" s="145"/>
-      <c r="B98" s="458" t="s">
+      <c r="B98" s="457" t="s">
         <v>36</v>
       </c>
-      <c r="C98" s="460"/>
-      <c r="D98" s="461"/>
-      <c r="E98" s="461"/>
-      <c r="F98" s="461"/>
-      <c r="G98" s="461"/>
-      <c r="H98" s="461"/>
-      <c r="I98" s="461"/>
-      <c r="J98" s="461"/>
-      <c r="K98" s="461"/>
-      <c r="L98" s="461"/>
-      <c r="M98" s="461"/>
-      <c r="N98" s="461"/>
-      <c r="O98" s="461"/>
-      <c r="P98" s="461"/>
-      <c r="Q98" s="461"/>
-      <c r="R98" s="461"/>
-      <c r="S98" s="461"/>
-      <c r="T98" s="461"/>
-      <c r="U98" s="461"/>
-      <c r="V98" s="461"/>
-      <c r="W98" s="461"/>
-      <c r="X98" s="461"/>
-      <c r="Y98" s="461"/>
-      <c r="Z98" s="461"/>
-      <c r="AA98" s="461"/>
-      <c r="AB98" s="462"/>
+      <c r="C98" s="459"/>
+      <c r="D98" s="460"/>
+      <c r="E98" s="460"/>
+      <c r="F98" s="460"/>
+      <c r="G98" s="460"/>
+      <c r="H98" s="460"/>
+      <c r="I98" s="460"/>
+      <c r="J98" s="460"/>
+      <c r="K98" s="460"/>
+      <c r="L98" s="460"/>
+      <c r="M98" s="460"/>
+      <c r="N98" s="460"/>
+      <c r="O98" s="460"/>
+      <c r="P98" s="460"/>
+      <c r="Q98" s="460"/>
+      <c r="R98" s="460"/>
+      <c r="S98" s="460"/>
+      <c r="T98" s="460"/>
+      <c r="U98" s="460"/>
+      <c r="V98" s="460"/>
+      <c r="W98" s="460"/>
+      <c r="X98" s="460"/>
+      <c r="Y98" s="460"/>
+      <c r="Z98" s="460"/>
+      <c r="AA98" s="460"/>
+      <c r="AB98" s="461"/>
       <c r="AC98" s="148"/>
       <c r="AD98" s="148"/>
       <c r="AE98" s="148"/>
@@ -20497,33 +20674,33 @@
     </row>
     <row r="99" spans="1:75" ht="28.5" customHeight="1">
       <c r="A99" s="145"/>
-      <c r="B99" s="458"/>
-      <c r="C99" s="463"/>
-      <c r="D99" s="464"/>
-      <c r="E99" s="464"/>
-      <c r="F99" s="464"/>
-      <c r="G99" s="464"/>
-      <c r="H99" s="464"/>
-      <c r="I99" s="464"/>
-      <c r="J99" s="464"/>
-      <c r="K99" s="464"/>
-      <c r="L99" s="464"/>
-      <c r="M99" s="464"/>
-      <c r="N99" s="464"/>
-      <c r="O99" s="464"/>
-      <c r="P99" s="464"/>
-      <c r="Q99" s="464"/>
-      <c r="R99" s="464"/>
-      <c r="S99" s="464"/>
-      <c r="T99" s="464"/>
-      <c r="U99" s="464"/>
-      <c r="V99" s="464"/>
-      <c r="W99" s="464"/>
-      <c r="X99" s="464"/>
-      <c r="Y99" s="464"/>
-      <c r="Z99" s="464"/>
-      <c r="AA99" s="464"/>
-      <c r="AB99" s="465"/>
+      <c r="B99" s="457"/>
+      <c r="C99" s="462"/>
+      <c r="D99" s="463"/>
+      <c r="E99" s="463"/>
+      <c r="F99" s="463"/>
+      <c r="G99" s="463"/>
+      <c r="H99" s="463"/>
+      <c r="I99" s="463"/>
+      <c r="J99" s="463"/>
+      <c r="K99" s="463"/>
+      <c r="L99" s="463"/>
+      <c r="M99" s="463"/>
+      <c r="N99" s="463"/>
+      <c r="O99" s="463"/>
+      <c r="P99" s="463"/>
+      <c r="Q99" s="463"/>
+      <c r="R99" s="463"/>
+      <c r="S99" s="463"/>
+      <c r="T99" s="463"/>
+      <c r="U99" s="463"/>
+      <c r="V99" s="463"/>
+      <c r="W99" s="463"/>
+      <c r="X99" s="463"/>
+      <c r="Y99" s="463"/>
+      <c r="Z99" s="463"/>
+      <c r="AA99" s="463"/>
+      <c r="AB99" s="464"/>
       <c r="AC99" s="148"/>
       <c r="AD99" s="148"/>
       <c r="AE99" s="148"/>
@@ -20534,7 +20711,7 @@
       <c r="AJ99" s="149"/>
       <c r="AP99" s="105"/>
     </row>
-    <row r="100" spans="1:75" ht="14.1" customHeight="1">
+    <row r="100" spans="1:75" ht="13.8" customHeight="1">
       <c r="M100" s="105"/>
       <c r="N100" s="105"/>
       <c r="O100" s="105"/>
@@ -20555,8 +20732,15 @@
       <c r="AP100" s="105"/>
     </row>
     <row r="101" spans="1:75" ht="14.1" customHeight="1">
-      <c r="K101" s="103"/>
-      <c r="L101" s="103"/>
+      <c r="C101" s="105"/>
+      <c r="D101" s="105"/>
+      <c r="E101" s="105"/>
+      <c r="F101" s="105"/>
+      <c r="G101" s="105"/>
+      <c r="H101" s="105"/>
+      <c r="I101" s="105"/>
+      <c r="J101" s="105"/>
+      <c r="K101" s="105"/>
       <c r="M101" s="105"/>
       <c r="N101" s="105"/>
       <c r="O101" s="105"/>
@@ -20602,8 +20786,21 @@
       <c r="BO101" s="103"/>
     </row>
     <row r="102" spans="1:75" ht="14.1" customHeight="1">
-      <c r="K102" s="103"/>
-      <c r="L102" s="103"/>
+      <c r="C102" s="501" t="s">
+        <v>593</v>
+      </c>
+      <c r="D102" s="501"/>
+      <c r="E102" s="105"/>
+      <c r="F102" s="501" t="s">
+        <v>594</v>
+      </c>
+      <c r="G102" s="501"/>
+      <c r="H102" s="105"/>
+      <c r="I102" s="501" t="s">
+        <v>595</v>
+      </c>
+      <c r="J102" s="501"/>
+      <c r="K102" s="105"/>
       <c r="M102" s="105"/>
       <c r="N102" s="105"/>
       <c r="O102" s="105"/>
@@ -20649,8 +20846,15 @@
       <c r="BO102" s="103"/>
     </row>
     <row r="103" spans="1:75" ht="14.1" customHeight="1">
-      <c r="K103" s="103"/>
-      <c r="L103" s="103"/>
+      <c r="C103" s="105"/>
+      <c r="D103" s="105"/>
+      <c r="E103" s="105"/>
+      <c r="F103" s="105"/>
+      <c r="G103" s="105"/>
+      <c r="H103" s="105"/>
+      <c r="I103" s="105"/>
+      <c r="J103" s="105"/>
+      <c r="K103" s="105"/>
       <c r="M103" s="105"/>
       <c r="N103" s="105"/>
       <c r="O103" s="105"/>
@@ -20695,7 +20899,7 @@
       <c r="BN103" s="103"/>
       <c r="BO103" s="103"/>
     </row>
-    <row r="104" spans="1:75" ht="14.1" customHeight="1">
+    <row r="104" spans="1:75" ht="13.8" customHeight="1">
       <c r="K104" s="103"/>
       <c r="L104" s="103"/>
       <c r="M104" s="105"/>
@@ -65347,7 +65551,10 @@
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0"/>
-  <mergeCells count="251">
+  <mergeCells count="254">
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="F102:G102"/>
+    <mergeCell ref="I102:J102"/>
     <mergeCell ref="C52:D52"/>
     <mergeCell ref="C53:D53"/>
     <mergeCell ref="A42:F42"/>
@@ -65420,6 +65627,18 @@
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="D17:D18"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="BF2:BS2"/>
+    <mergeCell ref="AG5:AJ5"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
@@ -65429,15 +65648,6 @@
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="D27:D28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="BF2:BS2"/>
-    <mergeCell ref="AG5:AJ5"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="E16:F16"/>
@@ -65462,9 +65672,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="E39:F39"/>
@@ -65609,20 +65816,12 @@
   <colBreaks count="1" manualBreakCount="1">
     <brk id="28" max="1048575" man="1"/>
   </colBreaks>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004D4CCBE22655944796F59B17B9006C15" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f481576c72d824a80c867b56d5274a41">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b7c6cbfa-29cf-4ada-90bf-db8e550dae8d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3bc755a260c778b5f630b987d93a78f8" ns2:_="">
     <xsd:import namespace="b7c6cbfa-29cf-4ada-90bf-db8e550dae8d"/>
@@ -65800,21 +65999,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5458833A-D997-4113-BB83-F938CBB9D86E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82807CA0-8C25-4FF6-8C67-D0A8F7400434}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -65832,7 +66032,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECA946AD-4EA3-4FCA-B864-262800288FDF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -65846,4 +66046,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5458833A-D997-4113-BB83-F938CBB9D86E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Pump and commingle issue fix in excelexport
</commit_message>
<xml_diff>
--- a/api/cp-dss-api/gateway/src/main/resources/reports/discharging/Vessel_1_Discharging_Plan_Template.xlsx
+++ b/api/cp-dss-api/gateway/src/main/resources/reports/discharging/Vessel_1_Discharging_Plan_Template.xlsx
@@ -3955,12 +3955,6 @@
     <t>${driveOilTank}</t>
   </si>
   <si>
-    <t>${sheetOne.berthDetails.maxManifoldPressure}</t>
-  </si>
-  <si>
-    <t>${sheetOne.berthDetails.airPurge}</t>
-  </si>
-  <si>
     <t>${berthDetails.berthName}</t>
   </si>
   <si>
@@ -4219,6 +4213,12 @@
   </si>
   <si>
     <t>${ballastPumpStatus2.colorCode}</t>
+  </si>
+  <si>
+    <t>${berthDetails.maxManifoldPressure}</t>
+  </si>
+  <si>
+    <t>${berthDetails.airPurge}</t>
   </si>
 </sst>
 </file>
@@ -7742,10 +7742,10 @@
           </xdr:nvGrpSpPr>
           <xdr:grpSpPr>
             <a:xfrm>
-              <a:off x="380552" y="3921619"/>
-              <a:ext cx="418203" cy="725634"/>
+              <a:off x="380552" y="3921607"/>
+              <a:ext cx="418203" cy="725643"/>
               <a:chOff x="376566" y="3942676"/>
-              <a:chExt cx="297180" cy="732365"/>
+              <a:chExt cx="297180" cy="732369"/>
             </a:xfrm>
           </xdr:grpSpPr>
           <xdr:sp macro="" textlink="">
@@ -7848,7 +7848,7 @@
             </xdr:nvSpPr>
             <xdr:spPr bwMode="auto">
               <a:xfrm>
-                <a:off x="392430" y="4404362"/>
+                <a:off x="392430" y="4404366"/>
                 <a:ext cx="243840" cy="270679"/>
               </a:xfrm>
               <a:prstGeom prst="rect">
@@ -8507,7 +8507,7 @@
       <c r="F7" s="338"/>
       <c r="G7" s="338"/>
       <c r="H7" s="339" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="I7" s="339"/>
       <c r="J7" s="338" t="s">
@@ -8685,7 +8685,7 @@
       <c r="N12" s="29"/>
       <c r="O12" s="29"/>
       <c r="P12" s="328" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="Q12" s="328"/>
       <c r="R12" s="328"/>
@@ -10539,7 +10539,7 @@
       <c r="G49" s="199"/>
       <c r="H49" s="200"/>
       <c r="I49" s="260" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="J49" s="260"/>
       <c r="K49" s="260"/>
@@ -10575,7 +10575,7 @@
       <c r="G50" s="199"/>
       <c r="H50" s="200"/>
       <c r="I50" s="260" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="J50" s="260"/>
       <c r="K50" s="260"/>
@@ -10609,7 +10609,7 @@
       <c r="G51" s="199"/>
       <c r="H51" s="200"/>
       <c r="I51" s="260" t="s">
-        <v>516</v>
+        <v>595</v>
       </c>
       <c r="J51" s="260"/>
       <c r="K51" s="260"/>
@@ -10643,7 +10643,7 @@
       <c r="G52" s="199"/>
       <c r="H52" s="200"/>
       <c r="I52" s="260" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="J52" s="260"/>
       <c r="K52" s="260"/>
@@ -10677,7 +10677,7 @@
       <c r="G53" s="199"/>
       <c r="H53" s="200"/>
       <c r="I53" s="260" t="s">
-        <v>517</v>
+        <v>596</v>
       </c>
       <c r="J53" s="260"/>
       <c r="K53" s="260"/>
@@ -10711,7 +10711,7 @@
       <c r="G54" s="268"/>
       <c r="H54" s="269"/>
       <c r="I54" s="259" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="J54" s="259"/>
       <c r="K54" s="259"/>
@@ -10980,7 +10980,7 @@
       <c r="D62" s="311"/>
       <c r="E62" s="312"/>
       <c r="F62" s="305" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="G62" s="306"/>
       <c r="H62" s="306"/>
@@ -11016,7 +11016,7 @@
       <c r="D63" s="196"/>
       <c r="E63" s="197"/>
       <c r="F63" s="308" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="G63" s="308"/>
       <c r="H63" s="308"/>
@@ -11052,7 +11052,7 @@
       <c r="D64" s="311"/>
       <c r="E64" s="312"/>
       <c r="F64" s="308" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="G64" s="308"/>
       <c r="H64" s="308"/>
@@ -11088,7 +11088,7 @@
       <c r="D65" s="311"/>
       <c r="E65" s="312"/>
       <c r="F65" s="308" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="G65" s="308"/>
       <c r="H65" s="308"/>
@@ -11124,7 +11124,7 @@
       <c r="D66" s="311"/>
       <c r="E66" s="312"/>
       <c r="F66" s="308" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="G66" s="308"/>
       <c r="H66" s="308"/>
@@ -11160,7 +11160,7 @@
       <c r="D67" s="311"/>
       <c r="E67" s="312"/>
       <c r="F67" s="308" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="G67" s="308"/>
       <c r="H67" s="308"/>
@@ -11196,7 +11196,7 @@
       <c r="D68" s="311"/>
       <c r="E68" s="312"/>
       <c r="F68" s="305" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="G68" s="306"/>
       <c r="H68" s="306"/>
@@ -11562,7 +11562,7 @@
       <c r="G2" s="347"/>
       <c r="H2" s="348"/>
       <c r="I2" s="352" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="J2" s="353"/>
       <c r="K2" s="353"/>
@@ -11619,10 +11619,10 @@
     <row r="4" spans="1:24" s="219" customFormat="1" ht="19.5" customHeight="1">
       <c r="A4" s="218"/>
       <c r="B4" s="253" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C4" s="364" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="D4" s="365"/>
       <c r="E4" s="365"/>
@@ -11630,28 +11630,28 @@
       <c r="G4" s="365"/>
       <c r="H4" s="366"/>
       <c r="I4" s="367" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="J4" s="368"/>
       <c r="K4" s="368"/>
       <c r="L4" s="369"/>
       <c r="M4" s="370" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="N4" s="371"/>
       <c r="O4" s="372"/>
       <c r="P4" s="373" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="Q4" s="374"/>
       <c r="R4" s="375" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="S4" s="376"/>
       <c r="T4" s="364"/>
       <c r="U4" s="366"/>
       <c r="V4" s="364" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="W4" s="365"/>
       <c r="X4" s="366"/>
@@ -11668,22 +11668,22 @@
       <c r="G5" s="378"/>
       <c r="H5" s="379"/>
       <c r="I5" s="380" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="J5" s="381"/>
       <c r="K5" s="381"/>
       <c r="L5" s="382"/>
       <c r="M5" s="383" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="N5" s="384"/>
       <c r="O5" s="385"/>
       <c r="P5" s="386" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="Q5" s="387"/>
       <c r="R5" s="388" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="S5" s="379"/>
       <c r="T5" s="377"/>
@@ -11730,18 +11730,18 @@
       <c r="G7" s="222"/>
       <c r="H7" s="223"/>
       <c r="I7" s="367" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="J7" s="368"/>
       <c r="K7" s="368"/>
       <c r="L7" s="369"/>
       <c r="M7" s="370" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="N7" s="371"/>
       <c r="O7" s="372"/>
       <c r="P7" s="373" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="Q7" s="374"/>
       <c r="R7" s="388"/>
@@ -11792,7 +11792,7 @@
       <c r="G10" s="231"/>
       <c r="H10" s="231"/>
       <c r="O10" s="346" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="P10" s="347"/>
       <c r="Q10" s="347"/>
@@ -11815,7 +11815,7 @@
       <c r="C11" s="232"/>
       <c r="D11" s="232"/>
       <c r="E11" s="400" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="F11" s="400"/>
       <c r="G11" s="400"/>
@@ -11826,7 +11826,7 @@
         <v>484</v>
       </c>
       <c r="L11" s="233" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="M11" s="250" t="s">
         <v>488</v>
@@ -11849,7 +11849,7 @@
       <c r="C12" s="232"/>
       <c r="D12" s="232"/>
       <c r="E12" s="393" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="F12" s="393"/>
       <c r="G12" s="393"/>
@@ -11860,24 +11860,24 @@
         <v>484</v>
       </c>
       <c r="L12" s="234" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="M12" s="250" t="s">
         <v>488</v>
       </c>
       <c r="O12" s="401" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="P12" s="402"/>
       <c r="Q12" s="402"/>
       <c r="R12" s="403"/>
       <c r="S12" s="389" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="T12" s="390"/>
       <c r="U12" s="391"/>
       <c r="V12" s="389" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="W12" s="390"/>
       <c r="X12" s="391"/>
@@ -11889,7 +11889,7 @@
       <c r="C13" s="392"/>
       <c r="D13" s="392"/>
       <c r="E13" s="393" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="F13" s="393"/>
       <c r="G13" s="393"/>
@@ -11900,7 +11900,7 @@
         <v>484</v>
       </c>
       <c r="L13" s="234" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="M13" s="250" t="s">
         <v>488</v>
@@ -11945,7 +11945,7 @@
         <v>8</v>
       </c>
       <c r="F15" s="405" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="G15" s="405"/>
       <c r="H15" s="405"/>
@@ -11975,7 +11975,7 @@
         <v>8</v>
       </c>
       <c r="F16" s="405" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="G16" s="405"/>
       <c r="H16" s="405"/>
@@ -12005,7 +12005,7 @@
         <v>498</v>
       </c>
       <c r="F17" s="405" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="G17" s="405"/>
       <c r="H17" s="405"/>
@@ -12055,7 +12055,7 @@
       <c r="E20" s="415"/>
       <c r="F20" s="424"/>
       <c r="G20" s="429" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="H20" s="430"/>
       <c r="I20" s="430"/>
@@ -12066,7 +12066,7 @@
         <v>502</v>
       </c>
       <c r="N20" s="412" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="O20" s="413"/>
       <c r="P20" s="239"/>
@@ -12076,7 +12076,7 @@
       <c r="R20" s="240"/>
       <c r="S20" s="241"/>
       <c r="T20" s="425" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="U20" s="425"/>
       <c r="V20" s="425"/>
@@ -12092,7 +12092,7 @@
       <c r="E21" s="410"/>
       <c r="F21" s="411"/>
       <c r="G21" s="429" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="H21" s="430"/>
       <c r="I21" s="430"/>
@@ -12103,7 +12103,7 @@
         <v>502</v>
       </c>
       <c r="N21" s="412" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="O21" s="413"/>
       <c r="P21" s="242"/>
@@ -12113,7 +12113,7 @@
       <c r="R21" s="243"/>
       <c r="S21" s="244"/>
       <c r="T21" s="426" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="U21" s="426" t="s">
         <v>506</v>
@@ -12135,7 +12135,7 @@
       <c r="E22" s="415"/>
       <c r="F22" s="245"/>
       <c r="G22" s="427" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="H22" s="428"/>
       <c r="I22" s="428"/>
@@ -12146,7 +12146,7 @@
         <v>502</v>
       </c>
       <c r="N22" s="412" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="O22" s="413"/>
       <c r="P22" s="416" t="s">
@@ -14262,7 +14262,7 @@
         <v>306</v>
       </c>
       <c r="E7" s="435" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="F7" s="436"/>
       <c r="G7" s="74"/>
@@ -14381,7 +14381,7 @@
         <v>310</v>
       </c>
       <c r="E9" s="435" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="F9" s="436"/>
       <c r="G9" s="74"/>
@@ -14501,7 +14501,7 @@
         <v>314</v>
       </c>
       <c r="E11" s="435" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="F11" s="436"/>
       <c r="G11" s="74"/>
@@ -14627,7 +14627,7 @@
         <v>318</v>
       </c>
       <c r="E13" s="435" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="F13" s="436"/>
       <c r="G13" s="74"/>
@@ -14753,7 +14753,7 @@
         <v>322</v>
       </c>
       <c r="E15" s="435" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="F15" s="436"/>
       <c r="G15" s="74"/>
@@ -14874,7 +14874,7 @@
         <v>326</v>
       </c>
       <c r="E17" s="435" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="F17" s="436"/>
       <c r="G17" s="74"/>
@@ -14998,7 +14998,7 @@
         <v>330</v>
       </c>
       <c r="E19" s="435" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="F19" s="436"/>
       <c r="G19" s="74"/>
@@ -15114,7 +15114,7 @@
         <v>334</v>
       </c>
       <c r="E21" s="435" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="F21" s="436"/>
       <c r="G21" s="74"/>
@@ -15230,7 +15230,7 @@
         <v>338</v>
       </c>
       <c r="E23" s="435" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F23" s="436"/>
       <c r="G23" s="74"/>
@@ -15346,7 +15346,7 @@
         <v>342</v>
       </c>
       <c r="E25" s="435" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="F25" s="436"/>
       <c r="G25" s="74"/>
@@ -15462,7 +15462,7 @@
         <v>346</v>
       </c>
       <c r="E27" s="435" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="F27" s="436"/>
       <c r="G27" s="74"/>
@@ -15578,7 +15578,7 @@
         <v>350</v>
       </c>
       <c r="E29" s="435" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F29" s="436"/>
       <c r="G29" s="74"/>
@@ -15694,7 +15694,7 @@
         <v>354</v>
       </c>
       <c r="E31" s="435" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="F31" s="436"/>
       <c r="G31" s="74"/>
@@ -15810,7 +15810,7 @@
         <v>358</v>
       </c>
       <c r="E33" s="435" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="F33" s="436"/>
       <c r="G33" s="74"/>
@@ -15926,7 +15926,7 @@
         <v>362</v>
       </c>
       <c r="E35" s="435" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="F35" s="436"/>
       <c r="G35" s="74"/>
@@ -16042,7 +16042,7 @@
         <v>366</v>
       </c>
       <c r="E37" s="435" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="F37" s="436"/>
       <c r="G37" s="74"/>
@@ -16158,7 +16158,7 @@
         <v>370</v>
       </c>
       <c r="E39" s="435" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="F39" s="436"/>
       <c r="G39" s="74"/>
@@ -16286,7 +16286,7 @@
     </row>
     <row r="41" spans="1:75" ht="22.2" customHeight="1">
       <c r="A41" s="483" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="B41" s="484"/>
       <c r="C41" s="484"/>
@@ -16365,7 +16365,7 @@
     </row>
     <row r="42" spans="1:75" ht="21.6" customHeight="1">
       <c r="A42" s="483" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B42" s="484"/>
       <c r="C42" s="484"/>
@@ -16373,7 +16373,7 @@
       <c r="E42" s="485"/>
       <c r="F42" s="486"/>
       <c r="G42" s="481" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="H42" s="482"/>
       <c r="I42" s="74"/>
@@ -16444,7 +16444,7 @@
     </row>
     <row r="43" spans="1:75" ht="37.799999999999997" customHeight="1">
       <c r="A43" s="508" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B43" s="509"/>
       <c r="C43" s="509"/>
@@ -16452,7 +16452,7 @@
       <c r="E43" s="509"/>
       <c r="F43" s="510"/>
       <c r="G43" s="504" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="H43" s="505"/>
       <c r="I43" s="74"/>
@@ -16531,7 +16531,7 @@
       </c>
       <c r="D44" s="447"/>
       <c r="E44" s="435" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="F44" s="436"/>
       <c r="G44" s="187"/>
@@ -16685,7 +16685,7 @@
       </c>
       <c r="D46" s="447"/>
       <c r="E46" s="435" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="F46" s="436"/>
       <c r="G46" s="187"/>
@@ -16839,7 +16839,7 @@
       </c>
       <c r="D48" s="447"/>
       <c r="E48" s="435" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="F48" s="436"/>
       <c r="G48" s="187"/>
@@ -16993,7 +16993,7 @@
       </c>
       <c r="D50" s="447"/>
       <c r="E50" s="435" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="F50" s="436"/>
       <c r="G50" s="187"/>
@@ -17147,7 +17147,7 @@
       </c>
       <c r="D52" s="447"/>
       <c r="E52" s="435" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="F52" s="436"/>
       <c r="G52" s="187"/>
@@ -19651,7 +19651,7 @@
       </c>
       <c r="D84" s="447"/>
       <c r="E84" s="437" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="F84" s="438"/>
       <c r="G84" s="74"/>
@@ -19732,7 +19732,7 @@
       </c>
       <c r="D85" s="447"/>
       <c r="E85" s="437" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="F85" s="438"/>
       <c r="G85" s="74"/>
@@ -19813,7 +19813,7 @@
       </c>
       <c r="D86" s="447"/>
       <c r="E86" s="437" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="F86" s="438"/>
       <c r="G86" s="74"/>
@@ -20787,17 +20787,17 @@
     </row>
     <row r="102" spans="1:75" ht="14.1" customHeight="1">
       <c r="C102" s="501" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="D102" s="501"/>
       <c r="E102" s="105"/>
       <c r="F102" s="501" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="G102" s="501"/>
       <c r="H102" s="105"/>
       <c r="I102" s="501" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="J102" s="501"/>
       <c r="K102" s="105"/>

</xml_diff>